<commit_message>
Fixed 49.3 and 50.10
</commit_message>
<xml_diff>
--- a/6.1_Merge_sample.xlsx
+++ b/6.1_Merge_sample.xlsx
@@ -8,17 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bomber\PycharmProjects\pythonProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A72F1A89-2CE4-48A1-B83A-2BF8E253D1EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E673A03-E46D-426C-952D-E991EF4019BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="49.1" sheetId="2" r:id="rId1"/>
     <sheet name="49.2" sheetId="3" r:id="rId2"/>
-    <sheet name="49.3" sheetId="4" r:id="rId3"/>
+    <sheet name="49.3" sheetId="13" r:id="rId3"/>
     <sheet name="49.4" sheetId="5" r:id="rId4"/>
     <sheet name="49.5" sheetId="6" r:id="rId5"/>
-    <sheet name="50.10" sheetId="7" r:id="rId6"/>
+    <sheet name="50.10" sheetId="14" r:id="rId6"/>
     <sheet name="50.2" sheetId="8" r:id="rId7"/>
     <sheet name="50.3" sheetId="9" r:id="rId8"/>
     <sheet name="50.4" sheetId="10" r:id="rId9"/>
@@ -408,7 +408,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -520,32 +520,32 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="6" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
@@ -2814,7 +2814,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:L76"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -8763,16 +8763,18 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0528EA5-9315-4EB1-A103-5A3B27DFD463}">
   <dimension ref="A1:L76"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="58.33203125" customWidth="1"/>
     <col min="2" max="2" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="13.77734375" style="3" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.5546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.5546875" bestFit="1" customWidth="1"/>
     <col min="11" max="12" width="10.21875" bestFit="1" customWidth="1"/>
@@ -8790,13 +8792,13 @@
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="G2" s="1" t="s">
@@ -8815,7 +8817,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="3" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>5</v>
       </c>
@@ -8836,13 +8838,14 @@
         <v>4.0216213245891285E-3</v>
       </c>
       <c r="H3" s="12">
-        <f t="shared" ref="H3:H12" si="0">D3/D$43</f>
+        <f t="shared" ref="H3:I12" si="0">D3/D$43</f>
         <v>3.3246591280154292E-3</v>
       </c>
       <c r="I3" s="12">
-        <f t="shared" ref="I3:I12" si="1">E3/E$43</f>
+        <f t="shared" si="0"/>
         <v>3.6078606050943041E-3</v>
       </c>
+      <c r="J3" s="3"/>
       <c r="K3" s="3">
         <f>C3-D3</f>
         <v>30892.350543665889</v>
@@ -8852,7 +8855,7 @@
         <v>2484.7514551981876</v>
       </c>
     </row>
-    <row r="4" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>7</v>
       </c>
@@ -8869,7 +8872,7 @@
         <v>0.93085367286619114</v>
       </c>
       <c r="G4" s="12">
-        <f t="shared" ref="G4:G12" si="2">C4/C$43</f>
+        <f t="shared" ref="G4:G12" si="1">C4/C$43</f>
         <v>1.1632476820247299E-7</v>
       </c>
       <c r="H4" s="12">
@@ -8877,19 +8880,20 @@
         <v>7.1239059577890064E-8</v>
       </c>
       <c r="I4" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3.8242913407313477E-8</v>
       </c>
+      <c r="J4" s="3"/>
       <c r="K4" s="3">
-        <f t="shared" ref="K4:K12" si="3">C4-D4</f>
+        <f t="shared" ref="K4:L12" si="2">C4-D4</f>
         <v>1.5705841091335708</v>
       </c>
       <c r="L4" s="3">
-        <f t="shared" ref="L4:L12" si="4">D4-E4</f>
+        <f t="shared" si="2"/>
         <v>1.0040920297648048</v>
       </c>
     </row>
-    <row r="5" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>9</v>
       </c>
@@ -8906,7 +8910,7 @@
         <v>3.117597615410291E-3</v>
       </c>
       <c r="G5" s="12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1.0252440159085864E-10</v>
       </c>
       <c r="H5" s="12">
@@ -8914,19 +8918,20 @@
         <v>1.1434146259141013E-10</v>
       </c>
       <c r="I5" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1.2808244638265645E-10</v>
       </c>
+      <c r="J5" s="3"/>
       <c r="K5" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>-1.60172166632222E-5</v>
       </c>
       <c r="L5" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>-1.1934472399657923E-5</v>
       </c>
     </row>
-    <row r="6" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>11</v>
       </c>
@@ -8943,7 +8948,7 @@
         <v>3.117597615410291E-3</v>
       </c>
       <c r="G6" s="12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1.0252440159085864E-10</v>
       </c>
       <c r="H6" s="12">
@@ -8951,19 +8956,20 @@
         <v>1.1434146259141013E-10</v>
       </c>
       <c r="I6" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1.2808244638265645E-10</v>
       </c>
+      <c r="J6" s="3"/>
       <c r="K6" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>-1.60172166632222E-5</v>
       </c>
       <c r="L6" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>-1.1934472399657923E-5</v>
       </c>
     </row>
-    <row r="7" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>13</v>
       </c>
@@ -8980,7 +8986,7 @@
         <v>22904258.18677767</v>
       </c>
       <c r="G7" s="12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0.91938225124991824</v>
       </c>
       <c r="H7" s="12">
@@ -8988,19 +8994,20 @@
         <v>0.93867278066896387</v>
       </c>
       <c r="I7" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.9409916811077591</v>
       </c>
+      <c r="J7" s="3"/>
       <c r="K7" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>2210663.4449013509</v>
       </c>
       <c r="L7" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>2591317.8903636485</v>
       </c>
     </row>
-    <row r="8" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>15</v>
       </c>
@@ -9017,7 +9024,7 @@
         <v>6557.9190225974862</v>
       </c>
       <c r="G8" s="12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>4.6788415638394909E-4</v>
       </c>
       <c r="H8" s="12">
@@ -9025,19 +9032,20 @@
         <v>2.5395958904207483E-4</v>
       </c>
       <c r="I8" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2.6942358033690735E-4</v>
       </c>
+      <c r="J8" s="3"/>
       <c r="K8" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>7202.1491643082281</v>
       </c>
       <c r="L8" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>339.95439643074587</v>
       </c>
     </row>
-    <row r="9" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>17</v>
       </c>
@@ -9054,7 +9062,7 @@
         <v>29380.254581318699</v>
       </c>
       <c r="G9" s="12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>3.301973733027369E-3</v>
       </c>
       <c r="H9" s="12">
@@ -9062,19 +9070,20 @@
         <v>1.0556566866164042E-3</v>
       </c>
       <c r="I9" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1.2070495767380509E-3</v>
       </c>
+      <c r="J9" s="3"/>
       <c r="K9" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>70834.320827575517</v>
       </c>
       <c r="L9" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>-707.24315577138987</v>
       </c>
     </row>
-    <row r="10" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
         <v>19</v>
       </c>
@@ -9091,7 +9100,7 @@
         <v>329266.4777946932</v>
       </c>
       <c r="G10" s="12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1.5604855135933245E-2</v>
       </c>
       <c r="H10" s="12">
@@ -9099,19 +9108,20 @@
         <v>1.4426317629725002E-2</v>
       </c>
       <c r="I10" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1.3527485323725693E-2</v>
       </c>
+      <c r="J10" s="3"/>
       <c r="K10" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>78425.845059671206</v>
       </c>
       <c r="L10" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>62571.110570800491</v>
       </c>
     </row>
-    <row r="11" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
         <v>21</v>
       </c>
@@ -9128,7 +9138,7 @@
         <v>44409.419176788768</v>
       </c>
       <c r="G11" s="12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1.3028445591976929E-2</v>
       </c>
       <c r="H11" s="12">
@@ -9136,19 +9146,20 @@
         <v>4.0367545165012333E-3</v>
       </c>
       <c r="I11" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1.8245032721605366E-3</v>
       </c>
+      <c r="J11" s="3"/>
       <c r="K11" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>282977.98153467628</v>
       </c>
       <c r="L11" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>65234.094515867226</v>
       </c>
     </row>
-    <row r="12" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>23</v>
       </c>
@@ -9165,7 +9176,7 @@
         <v>23401690.5178679</v>
       </c>
       <c r="G12" s="13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0.95580714772164588</v>
       </c>
       <c r="H12" s="13">
@@ -9173,23 +9184,30 @@
         <v>0.96177019968660626</v>
       </c>
       <c r="I12" s="13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.96142804196489284</v>
       </c>
+      <c r="J12" s="11"/>
       <c r="K12" s="11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>2680997.6625833288</v>
       </c>
       <c r="L12" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>2721241.5622143298</v>
       </c>
     </row>
-    <row r="13" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="4"/>
       <c r="B13" s="2"/>
-    </row>
-    <row r="14" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
         <v>25</v>
       </c>
@@ -9206,27 +9224,28 @@
         <v>143760.391649064</v>
       </c>
       <c r="G14" s="12">
-        <f t="shared" ref="G14:G20" si="5">C14/C$43</f>
+        <f t="shared" ref="G14:I20" si="3">C14/C$43</f>
         <v>7.4513810604479244E-3</v>
       </c>
       <c r="H14" s="12">
-        <f t="shared" ref="H14:H20" si="6">D14/D$43</f>
+        <f t="shared" si="3"/>
         <v>7.3607933636697731E-3</v>
       </c>
       <c r="I14" s="12">
-        <f t="shared" ref="I14:I20" si="7">E14/E$43</f>
+        <f t="shared" si="3"/>
         <v>5.9062088591306759E-3</v>
       </c>
+      <c r="J14" s="3"/>
       <c r="K14" s="3">
-        <f t="shared" ref="K14:K20" si="8">C14-D14</f>
+        <f t="shared" ref="K14:L20" si="4">C14-D14</f>
         <v>24623.939027770917</v>
       </c>
       <c r="L14" s="3">
-        <f t="shared" ref="L14:L20" si="9">D14-E14</f>
+        <f t="shared" si="4"/>
         <v>56168.349288554891</v>
       </c>
     </row>
-    <row r="15" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
         <v>27</v>
       </c>
@@ -9243,27 +9262,28 @@
         <v>11463.12964953795</v>
       </c>
       <c r="G15" s="12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>1.7622192762174133E-4</v>
       </c>
       <c r="H15" s="12">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>1.3725973829793801E-4</v>
       </c>
       <c r="I15" s="12">
-        <f t="shared" si="7"/>
+        <f t="shared" si="3"/>
         <v>4.7094778410688455E-4</v>
       </c>
+      <c r="J15" s="3"/>
       <c r="K15" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="4"/>
         <v>1582.4200283407722</v>
       </c>
       <c r="L15" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="4"/>
         <v>-7734.9762693903049</v>
       </c>
     </row>
-    <row r="16" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
         <v>29</v>
       </c>
@@ -9280,27 +9300,28 @@
         <v>229136.61409036821</v>
       </c>
       <c r="G16" s="12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>1.3153113698378936E-2</v>
       </c>
       <c r="H16" s="12">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>1.1187918690687236E-2</v>
       </c>
       <c r="I16" s="12">
-        <f t="shared" si="7"/>
+        <f t="shared" si="3"/>
         <v>9.4137800027379853E-3</v>
       </c>
+      <c r="J16" s="3"/>
       <c r="K16" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="4"/>
         <v>92500.004845072341</v>
       </c>
       <c r="L16" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="4"/>
         <v>74741.838547838677</v>
       </c>
     </row>
-    <row r="17" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" s="6" t="s">
         <v>31</v>
       </c>
@@ -9317,27 +9338,28 @@
         <v>32075.501522137682</v>
       </c>
       <c r="G17" s="12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>1.1738488574113087E-3</v>
       </c>
       <c r="H17" s="12">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>1.2814295584657462E-3</v>
       </c>
       <c r="I17" s="12">
-        <f t="shared" si="7"/>
+        <f t="shared" si="3"/>
         <v>1.317780294544311E-3</v>
       </c>
+      <c r="J17" s="3"/>
       <c r="K17" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="4"/>
         <v>569.47522454163845</v>
       </c>
       <c r="L17" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="4"/>
         <v>2729.7953482771118</v>
       </c>
     </row>
-    <row r="18" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
         <v>33</v>
       </c>
@@ -9354,27 +9376,28 @@
         <v>507436.62853445078</v>
       </c>
       <c r="G18" s="12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>2.1707363390011451E-2</v>
       </c>
       <c r="H18" s="12">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>1.777480242618841E-2</v>
       </c>
       <c r="I18" s="12">
-        <f t="shared" si="7"/>
+        <f t="shared" si="3"/>
         <v>2.0847374415991222E-2</v>
       </c>
+      <c r="J18" s="3"/>
       <c r="K18" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="4"/>
         <v>171380.07037486666</v>
       </c>
       <c r="L18" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="4"/>
         <v>-24649.82908121025</v>
       </c>
     </row>
-    <row r="19" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" s="6" t="s">
         <v>35</v>
       </c>
@@ -9391,27 +9414,28 @@
         <v>14990.535727786861</v>
       </c>
       <c r="G19" s="12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>5.3092334448261093E-4</v>
       </c>
       <c r="H19" s="12">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>4.8759653608460019E-4</v>
       </c>
       <c r="I19" s="12">
-        <f t="shared" si="7"/>
+        <f t="shared" si="3"/>
         <v>6.1586667859600346E-4</v>
       </c>
+      <c r="J19" s="3"/>
       <c r="K19" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="4"/>
         <v>2755.9960588650702</v>
       </c>
       <c r="L19" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="4"/>
         <v>-1746.7783325464115</v>
       </c>
     </row>
-    <row r="20" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
         <v>37</v>
       </c>
@@ -9428,31 +9452,38 @@
         <v>938862.80117334542</v>
       </c>
       <c r="G20" s="13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>4.4192852278353956E-2</v>
       </c>
       <c r="H20" s="13">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>3.8229800313393694E-2</v>
       </c>
       <c r="I20" s="13">
-        <f t="shared" si="7"/>
+        <f t="shared" si="3"/>
         <v>3.857195803510708E-2</v>
       </c>
+      <c r="J20" s="11"/>
       <c r="K20" s="11">
-        <f t="shared" si="8"/>
+        <f t="shared" si="4"/>
         <v>293411.90555945702</v>
       </c>
       <c r="L20" s="11">
-        <f t="shared" si="9"/>
+        <f t="shared" si="4"/>
         <v>99508.399501523585</v>
       </c>
     </row>
-    <row r="21" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" s="4"/>
       <c r="B21" s="2"/>
-    </row>
-    <row r="22" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="3"/>
+      <c r="L21" s="3"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" s="6" t="s">
         <v>39</v>
       </c>
@@ -9469,27 +9500,28 @@
         <v>2216774.6684127338</v>
       </c>
       <c r="G22" s="12">
-        <f t="shared" ref="G22:G28" si="10">C22/C$43</f>
+        <f t="shared" ref="G22:I28" si="5">C22/C$43</f>
         <v>8.6285274465680892E-2</v>
       </c>
       <c r="H22" s="12">
-        <f t="shared" ref="H22:H28" si="11">D22/D$43</f>
+        <f t="shared" si="5"/>
         <v>8.9948991884934645E-2</v>
       </c>
       <c r="I22" s="12">
-        <f t="shared" ref="I22:I28" si="12">E22/E$43</f>
+        <f t="shared" si="5"/>
         <v>9.1073306319564409E-2</v>
       </c>
+      <c r="J22" s="3"/>
       <c r="K22" s="3">
-        <f t="shared" ref="K22:K28" si="13">C22-D22</f>
+        <f t="shared" ref="K22:L28" si="6">C22-D22</f>
         <v>157136.40600120416</v>
       </c>
       <c r="L22" s="3">
-        <f t="shared" ref="L22:L28" si="14">D22-E22</f>
+        <f t="shared" si="6"/>
         <v>226357.17997233523</v>
       </c>
     </row>
-    <row r="23" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
         <v>41</v>
       </c>
@@ -9506,27 +9538,28 @@
         <v>2.7683918034276229E-3</v>
       </c>
       <c r="G23" s="12">
-        <f t="shared" si="10"/>
+        <f t="shared" si="5"/>
         <v>3.8959392623146781E-9</v>
       </c>
       <c r="H23" s="12">
-        <f t="shared" si="11"/>
+        <f t="shared" si="5"/>
         <v>-8.8121479620320195E-7</v>
       </c>
       <c r="I23" s="12">
-        <f t="shared" si="12"/>
+        <f t="shared" si="5"/>
         <v>1.1373577942708277E-10</v>
       </c>
+      <c r="J23" s="3"/>
       <c r="K23" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="6"/>
         <v>24.052349242051598</v>
       </c>
       <c r="L23" s="3">
-        <f t="shared" si="14"/>
+        <f t="shared" si="6"/>
         <v>-23.937710726969158</v>
       </c>
     </row>
-    <row r="24" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" s="6" t="s">
         <v>43</v>
       </c>
@@ -9543,27 +9576,28 @@
         <v>6387406.8066617921</v>
       </c>
       <c r="G24" s="12">
-        <f t="shared" si="10"/>
+        <f t="shared" si="5"/>
         <v>5.6458755394367149E-2</v>
       </c>
       <c r="H24" s="12">
-        <f t="shared" si="11"/>
+        <f t="shared" si="5"/>
         <v>5.6714267142570621E-2</v>
       </c>
       <c r="I24" s="12">
-        <f t="shared" si="12"/>
+        <f t="shared" si="5"/>
         <v>0.26241830754377388</v>
       </c>
+      <c r="J24" s="3"/>
       <c r="K24" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="6"/>
         <v>160991.43016568804</v>
       </c>
       <c r="L24" s="3">
-        <f t="shared" si="14"/>
+        <f t="shared" si="6"/>
         <v>-4846973.3964565545</v>
       </c>
     </row>
-    <row r="25" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" s="6" t="s">
         <v>45</v>
       </c>
@@ -9580,27 +9614,28 @@
         <v>5099367.7491084673</v>
       </c>
       <c r="G25" s="12">
-        <f t="shared" si="10"/>
+        <f t="shared" si="5"/>
         <v>0.27152399918847803</v>
       </c>
       <c r="H25" s="12">
-        <f t="shared" si="11"/>
+        <f t="shared" si="5"/>
         <v>0.24204355169028896</v>
       </c>
       <c r="I25" s="12">
-        <f t="shared" si="12"/>
+        <f t="shared" si="5"/>
         <v>0.20950089680661896</v>
       </c>
+      <c r="J25" s="3"/>
       <c r="K25" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="6"/>
         <v>1608350.9565173555</v>
       </c>
       <c r="L25" s="3">
-        <f t="shared" si="14"/>
+        <f t="shared" si="6"/>
         <v>1474850.5655030785</v>
       </c>
     </row>
-    <row r="26" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26" s="6" t="s">
         <v>47</v>
       </c>
@@ -9617,27 +9652,28 @@
         <v>6189.0500412415713</v>
       </c>
       <c r="G26" s="12">
-        <f t="shared" si="10"/>
+        <f t="shared" si="5"/>
         <v>2.2718266024369948E-4</v>
       </c>
       <c r="H26" s="12">
-        <f t="shared" si="11"/>
+        <f t="shared" si="5"/>
         <v>2.3934168820355508E-4</v>
       </c>
       <c r="I26" s="12">
-        <f t="shared" si="12"/>
+        <f t="shared" si="5"/>
         <v>2.5426907762199352E-4</v>
       </c>
+      <c r="J26" s="3"/>
       <c r="K26" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="6"/>
         <v>345.47923232814901</v>
       </c>
       <c r="L26" s="3">
-        <f t="shared" si="14"/>
+        <f t="shared" si="6"/>
         <v>311.78213978359236</v>
       </c>
     </row>
-    <row r="27" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" s="6" t="s">
         <v>49</v>
       </c>
@@ -9654,27 +9690,28 @@
         <v>-188353.36069323131</v>
       </c>
       <c r="G27" s="12">
-        <f t="shared" si="10"/>
+        <f t="shared" si="5"/>
         <v>0.12763649841873864</v>
       </c>
       <c r="H27" s="12">
-        <f t="shared" si="11"/>
+        <f t="shared" si="5"/>
         <v>0.1613659353958416</v>
       </c>
       <c r="I27" s="12">
-        <f t="shared" si="12"/>
+        <f t="shared" si="5"/>
         <v>-7.7382530390500744E-3</v>
       </c>
+      <c r="J27" s="3"/>
       <c r="K27" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="6"/>
         <v>-536492.24508333858</v>
       </c>
       <c r="L27" s="3">
-        <f t="shared" si="14"/>
+        <f t="shared" si="6"/>
         <v>4571262.471162742</v>
       </c>
     </row>
-    <row r="28" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
         <v>51</v>
       </c>
@@ -9691,31 +9728,38 @@
         <v>13521384.916299401</v>
       </c>
       <c r="G28" s="13">
-        <f t="shared" si="10"/>
+        <f t="shared" si="5"/>
         <v>0.54213171402344762</v>
       </c>
       <c r="H28" s="13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="5"/>
         <v>0.55031120658704302</v>
       </c>
       <c r="I28" s="13">
-        <f t="shared" si="12"/>
+        <f t="shared" si="5"/>
         <v>0.55550852682226515</v>
       </c>
+      <c r="J28" s="11"/>
       <c r="K28" s="11">
-        <f t="shared" si="13"/>
+        <f t="shared" si="6"/>
         <v>1390356.0791824814</v>
       </c>
       <c r="L28" s="11">
-        <f t="shared" si="14"/>
+        <f t="shared" si="6"/>
         <v>1425784.6646106485</v>
       </c>
     </row>
-    <row r="29" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" s="4"/>
       <c r="B29" s="2"/>
-    </row>
-    <row r="30" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+      <c r="I29" s="3"/>
+      <c r="J29" s="3"/>
+      <c r="K29" s="3"/>
+      <c r="L29" s="3"/>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" s="6" t="s">
         <v>53</v>
       </c>
@@ -9732,27 +9776,28 @@
         <v>213315.36934597019</v>
       </c>
       <c r="G30" s="12">
-        <f t="shared" ref="G30:G34" si="15">C30/C$43</f>
+        <f t="shared" ref="G30:I34" si="7">C30/C$43</f>
         <v>9.4394398171904533E-3</v>
       </c>
       <c r="H30" s="12">
-        <f t="shared" ref="H30:H34" si="16">D30/D$43</f>
+        <f t="shared" si="7"/>
         <v>8.2578467218703648E-3</v>
       </c>
       <c r="I30" s="12">
-        <f t="shared" ref="I30:I34" si="17">E30/E$43</f>
+        <f t="shared" si="7"/>
         <v>8.7637847237883783E-3</v>
       </c>
+      <c r="J30" s="3"/>
       <c r="K30" s="3">
-        <f t="shared" ref="K30:K34" si="18">C30-D30</f>
+        <f t="shared" ref="K30:L34" si="8">C30-D30</f>
         <v>60170.36852659678</v>
       </c>
       <c r="L30" s="3">
-        <f t="shared" ref="L30:L34" si="19">D30-E30</f>
+        <f t="shared" si="8"/>
         <v>10978.509912756621</v>
       </c>
     </row>
-    <row r="31" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31" s="6" t="s">
         <v>55</v>
       </c>
@@ -9769,27 +9814,28 @@
         <v>2152584.348722891</v>
       </c>
       <c r="G31" s="12">
-        <f t="shared" si="15"/>
+        <f t="shared" si="7"/>
         <v>7.3855996964745999E-2</v>
       </c>
       <c r="H31" s="12">
-        <f t="shared" si="16"/>
+        <f t="shared" si="7"/>
         <v>8.4432996012555439E-2</v>
       </c>
       <c r="I31" s="12">
-        <f t="shared" si="17"/>
+        <f t="shared" si="7"/>
         <v>8.8436130457188775E-2</v>
       </c>
+      <c r="J31" s="3"/>
       <c r="K31" s="3">
-        <f t="shared" si="18"/>
+        <f t="shared" si="8"/>
         <v>-67607.094901165925</v>
       </c>
       <c r="L31" s="3">
-        <f t="shared" si="19"/>
+        <f t="shared" si="8"/>
         <v>140725.86287708208</v>
       </c>
     </row>
-    <row r="32" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32" s="6" t="s">
         <v>57</v>
       </c>
@@ -9806,27 +9852,28 @@
         <v>2353.4077722728171</v>
       </c>
       <c r="G32" s="12">
-        <f t="shared" si="15"/>
+        <f t="shared" si="7"/>
         <v>1.6669540870627663E-4</v>
       </c>
       <c r="H32" s="12">
-        <f t="shared" si="16"/>
+        <f t="shared" si="7"/>
         <v>1.3973369706900108E-4</v>
       </c>
       <c r="I32" s="12">
-        <f t="shared" si="17"/>
+        <f t="shared" si="7"/>
         <v>9.6686699822546012E-5</v>
       </c>
+      <c r="J32" s="3"/>
       <c r="K32" s="3">
-        <f t="shared" si="18"/>
+        <f t="shared" si="8"/>
         <v>1228.1356453697808</v>
       </c>
       <c r="L32" s="3">
-        <f t="shared" si="19"/>
+        <f t="shared" si="8"/>
         <v>1441.9415523597609</v>
       </c>
     </row>
-    <row r="33" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33" s="6" t="s">
         <v>59</v>
       </c>
@@ -9843,27 +9890,28 @@
         <v>1196558.9846792901</v>
       </c>
       <c r="G33" s="12">
-        <f t="shared" si="15"/>
+        <f t="shared" si="7"/>
         <v>6.1788877803503214E-2</v>
       </c>
       <c r="H33" s="12">
-        <f t="shared" si="16"/>
+        <f t="shared" si="7"/>
         <v>6.2322921787605852E-2</v>
       </c>
       <c r="I33" s="12">
-        <f t="shared" si="17"/>
+        <f t="shared" si="7"/>
         <v>4.9159070831115412E-2</v>
       </c>
+      <c r="J33" s="3"/>
       <c r="K33" s="3">
-        <f t="shared" si="18"/>
+        <f t="shared" si="8"/>
         <v>169280.09872607002</v>
       </c>
       <c r="L33" s="3">
-        <f t="shared" si="19"/>
+        <f t="shared" si="8"/>
         <v>496212.79533677688</v>
       </c>
     </row>
-    <row r="34" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:12" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="4" t="s">
         <v>61</v>
       </c>
@@ -9880,31 +9928,38 @@
         <v>3564812.1105204239</v>
       </c>
       <c r="G34" s="13">
-        <f t="shared" si="15"/>
+        <f t="shared" si="7"/>
         <v>0.14525100999414592</v>
       </c>
       <c r="H34" s="13">
-        <f t="shared" si="16"/>
+        <f t="shared" si="7"/>
         <v>0.15515349821910066</v>
       </c>
       <c r="I34" s="13">
-        <f t="shared" si="17"/>
+        <f t="shared" si="7"/>
         <v>0.14645567271191509</v>
       </c>
+      <c r="J34" s="11"/>
       <c r="K34" s="11">
-        <f t="shared" si="18"/>
+        <f t="shared" si="8"/>
         <v>163071.5079968702</v>
       </c>
       <c r="L34" s="11">
-        <f t="shared" si="19"/>
+        <f t="shared" si="8"/>
         <v>649359.10967897577</v>
       </c>
     </row>
-    <row r="35" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A35" s="4"/>
       <c r="B35" s="2"/>
-    </row>
-    <row r="36" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G35" s="3"/>
+      <c r="H35" s="3"/>
+      <c r="I35" s="3"/>
+      <c r="J35" s="3"/>
+      <c r="K35" s="3"/>
+      <c r="L35" s="3"/>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A36" s="6" t="s">
         <v>53</v>
       </c>
@@ -9921,27 +9976,28 @@
         <v>103592.1556983544</v>
       </c>
       <c r="G36" s="12">
-        <f t="shared" ref="G36:G41" si="20">C36/C$43</f>
+        <f t="shared" ref="G36:I41" si="9">C36/C$43</f>
         <v>6.400179064881082E-3</v>
       </c>
       <c r="H36" s="12">
-        <f t="shared" ref="H36:H41" si="21">D36/D$43</f>
+        <f t="shared" si="9"/>
         <v>4.1717591289620057E-3</v>
       </c>
       <c r="I36" s="12">
-        <f t="shared" ref="I36:I41" si="22">E36/E$43</f>
+        <f t="shared" si="9"/>
         <v>4.2559490879492791E-3</v>
       </c>
+      <c r="J36" s="3"/>
       <c r="K36" s="3">
-        <f t="shared" ref="K36:K41" si="23">C36-D36</f>
+        <f t="shared" ref="K36:L41" si="10">C36-D36</f>
         <v>79563.543564792795</v>
       </c>
       <c r="L36" s="3">
-        <f t="shared" ref="L36:L41" si="24">D36-E36</f>
+        <f t="shared" si="10"/>
         <v>9718.2592176496983</v>
       </c>
     </row>
-    <row r="37" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37" s="6" t="s">
         <v>64</v>
       </c>
@@ -9958,27 +10014,28 @@
         <v>473619.1784096997</v>
       </c>
       <c r="G37" s="12">
-        <f t="shared" si="20"/>
+        <f t="shared" si="9"/>
         <v>2.163823390527007E-2</v>
       </c>
       <c r="H37" s="12">
-        <f t="shared" si="21"/>
+        <f t="shared" si="9"/>
         <v>1.8474435982237504E-2</v>
       </c>
       <c r="I37" s="12">
-        <f t="shared" si="22"/>
+        <f t="shared" si="9"/>
         <v>1.9458028426954228E-2</v>
       </c>
+      <c r="J37" s="3"/>
       <c r="K37" s="3">
-        <f t="shared" si="23"/>
+        <f t="shared" si="10"/>
         <v>150293.84487206396</v>
       </c>
       <c r="L37" s="3">
-        <f t="shared" si="24"/>
+        <f t="shared" si="10"/>
         <v>28170.580244784825</v>
       </c>
     </row>
-    <row r="38" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A38" s="6" t="s">
         <v>66</v>
       </c>
@@ -9995,27 +10052,28 @@
         <v>108322.7865498905</v>
       </c>
       <c r="G38" s="12">
-        <f t="shared" si="20"/>
+        <f t="shared" si="9"/>
         <v>6.9192758183929922E-3</v>
       </c>
       <c r="H38" s="12">
-        <f t="shared" si="21"/>
+        <f t="shared" si="9"/>
         <v>6.5534138478240654E-3</v>
       </c>
       <c r="I38" s="12">
-        <f t="shared" si="22"/>
+        <f t="shared" si="9"/>
         <v>4.4503009085315745E-3</v>
       </c>
+      <c r="J38" s="3"/>
       <c r="K38" s="3">
-        <f t="shared" si="23"/>
+        <f t="shared" si="10"/>
         <v>30518.048140365194</v>
       </c>
       <c r="L38" s="3">
-        <f t="shared" si="24"/>
+        <f t="shared" si="10"/>
         <v>69676.474495172297</v>
       </c>
     </row>
-    <row r="39" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A39" s="6" t="s">
         <v>57</v>
       </c>
@@ -10032,27 +10090,28 @@
         <v>72127.066958678683</v>
       </c>
       <c r="G39" s="12">
-        <f t="shared" si="20"/>
+        <f t="shared" si="9"/>
         <v>2.9664503883270778E-3</v>
       </c>
       <c r="H39" s="12">
-        <f t="shared" si="21"/>
+        <f t="shared" si="9"/>
         <v>2.8479905242507117E-3</v>
       </c>
       <c r="I39" s="12">
-        <f t="shared" si="22"/>
+        <f t="shared" si="9"/>
         <v>2.963246809276713E-3</v>
       </c>
+      <c r="J39" s="3"/>
       <c r="K39" s="3">
-        <f t="shared" si="23"/>
+        <f t="shared" si="10"/>
         <v>12040.962713236397</v>
       </c>
       <c r="L39" s="3">
-        <f t="shared" si="24"/>
+        <f t="shared" si="10"/>
         <v>5228.0674112173001</v>
       </c>
     </row>
-    <row r="40" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A40" s="6" t="s">
         <v>59</v>
       </c>
@@ -10069,27 +10128,28 @@
         <v>6496695.1046048012</v>
       </c>
       <c r="G40" s="12">
-        <f t="shared" si="20"/>
+        <f t="shared" si="9"/>
         <v>0.2746931368055352</v>
       </c>
       <c r="H40" s="12">
-        <f t="shared" si="21"/>
+        <f t="shared" si="9"/>
         <v>0.26248769571058178</v>
       </c>
       <c r="I40" s="12">
-        <f t="shared" si="22"/>
+        <f t="shared" si="9"/>
         <v>0.26690827523310795</v>
       </c>
+      <c r="J40" s="3"/>
       <c r="K40" s="3">
-        <f t="shared" si="23"/>
+        <f t="shared" si="10"/>
         <v>1148565.5816729851</v>
       </c>
       <c r="L40" s="3">
-        <f t="shared" si="24"/>
+        <f t="shared" si="10"/>
         <v>632812.80605739541</v>
       </c>
     </row>
-    <row r="41" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:12" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A41" s="4" t="s">
         <v>70</v>
       </c>
@@ -10106,31 +10166,38 @@
         <v>7254356.2922214242</v>
       </c>
       <c r="G41" s="13">
-        <f t="shared" si="20"/>
+        <f t="shared" si="9"/>
         <v>0.31261727598240641</v>
       </c>
       <c r="H41" s="13">
-        <f t="shared" si="21"/>
+        <f t="shared" si="9"/>
         <v>0.29453529519385607</v>
       </c>
       <c r="I41" s="13">
-        <f t="shared" si="22"/>
+        <f t="shared" si="9"/>
         <v>0.29803580046581973</v>
       </c>
+      <c r="J41" s="11"/>
       <c r="K41" s="11">
-        <f t="shared" si="23"/>
+        <f t="shared" si="10"/>
         <v>1420981.9809634443</v>
       </c>
       <c r="L41" s="11">
-        <f t="shared" si="24"/>
+        <f t="shared" si="10"/>
         <v>745606.18742621969</v>
       </c>
     </row>
-    <row r="42" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A42" s="4"/>
       <c r="B42" s="2"/>
-    </row>
-    <row r="43" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G42" s="3"/>
+      <c r="H42" s="3"/>
+      <c r="I42" s="3"/>
+      <c r="J42" s="3"/>
+      <c r="K42" s="3"/>
+      <c r="L42" s="3"/>
+    </row>
+    <row r="43" spans="1:12" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A43" s="4" t="s">
         <v>72</v>
       </c>
@@ -10146,16 +10213,20 @@
       <c r="E43" s="11">
         <v>24340553.319041248</v>
       </c>
+      <c r="G43" s="11"/>
+      <c r="H43" s="11"/>
+      <c r="I43" s="11"/>
+      <c r="J43" s="11"/>
       <c r="K43" s="11">
-        <f t="shared" ref="K43:K63" si="25">C43-D43</f>
+        <f t="shared" ref="K43:L63" si="11">C43-D43</f>
         <v>2974409.5681427903</v>
       </c>
       <c r="L43" s="11">
-        <f t="shared" ref="L43:L44" si="26">D43-E43</f>
+        <f t="shared" si="11"/>
         <v>2820749.961715851</v>
       </c>
     </row>
-    <row r="44" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:12" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A44" s="4" t="s">
         <v>74</v>
       </c>
@@ -10171,20 +10242,30 @@
       <c r="E44" s="11">
         <v>24340553.319041248</v>
       </c>
+      <c r="G44" s="11"/>
+      <c r="H44" s="11"/>
+      <c r="I44" s="11"/>
+      <c r="J44" s="11"/>
       <c r="K44" s="11">
-        <f t="shared" si="25"/>
+        <f t="shared" si="11"/>
         <v>2974409.5681427903</v>
       </c>
       <c r="L44" s="11">
-        <f t="shared" si="26"/>
+        <f t="shared" si="11"/>
         <v>2820749.961715851</v>
       </c>
     </row>
-    <row r="45" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A45" s="4"/>
       <c r="B45" s="2"/>
-    </row>
-    <row r="46" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G45" s="3"/>
+      <c r="H45" s="3"/>
+      <c r="I45" s="3"/>
+      <c r="J45" s="3"/>
+      <c r="K45" s="3"/>
+      <c r="L45" s="3"/>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A46" s="6" t="s">
         <v>76</v>
       </c>
@@ -10195,22 +10276,28 @@
         <v>2615179.0406829002</v>
       </c>
       <c r="D46" s="3">
-        <v>2192074.8317521471</v>
+        <v>2186784.9755981052</v>
+      </c>
+      <c r="E46" s="3">
+        <v>0</v>
       </c>
       <c r="G46" s="12">
         <f>C$63/C46</f>
         <v>-3.9782418965019224E-2</v>
       </c>
       <c r="H46" s="12">
-        <f t="shared" ref="H46:H48" si="27">D$63/D46</f>
-        <v>-6.3643989699523465E-2</v>
-      </c>
+        <f t="shared" ref="H46:H48" si="12">D$63/D46</f>
+        <v>-6.3797945188671518E-2</v>
+      </c>
+      <c r="I46" s="3"/>
+      <c r="J46" s="3"/>
       <c r="K46" s="3">
-        <f t="shared" si="25"/>
-        <v>423104.20893075317</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+        <f t="shared" si="11"/>
+        <v>428394.065084795</v>
+      </c>
+      <c r="L46" s="3"/>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A47" s="6" t="s">
         <v>78</v>
       </c>
@@ -10221,22 +10308,28 @@
         <v>2751681.6956907641</v>
       </c>
       <c r="D47" s="3">
-        <v>2419007.5278316909</v>
+        <v>2413170.04378579</v>
+      </c>
+      <c r="E47" s="3">
+        <v>0</v>
       </c>
       <c r="G47" s="12">
-        <f t="shared" ref="G47:G48" si="28">C$63/C47</f>
+        <f t="shared" ref="G47:G48" si="13">C$63/C47</f>
         <v>-3.780893278023828E-2</v>
       </c>
       <c r="H47" s="12">
-        <f t="shared" si="27"/>
-        <v>-5.7673399692836858E-2</v>
-      </c>
+        <f t="shared" si="12"/>
+        <v>-5.7812912261147889E-2</v>
+      </c>
+      <c r="I47" s="3"/>
+      <c r="J47" s="3"/>
       <c r="K47" s="3">
-        <f t="shared" si="25"/>
-        <v>332674.16785907326</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.3">
+        <f t="shared" si="11"/>
+        <v>338511.65190497413</v>
+      </c>
+      <c r="L47" s="3"/>
+    </row>
+    <row r="48" spans="1:12" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A48" s="4" t="s">
         <v>80</v>
       </c>
@@ -10247,26 +10340,38 @@
         <v>-136502.65500786441</v>
       </c>
       <c r="D48" s="11">
-        <v>-226932.69607954411</v>
+        <v>-226385.06818768501</v>
+      </c>
+      <c r="E48" s="11">
+        <v>0</v>
       </c>
       <c r="G48" s="14">
-        <f t="shared" si="28"/>
+        <f t="shared" si="13"/>
         <v>0.76216941171576613</v>
       </c>
       <c r="H48" s="14">
-        <f t="shared" si="27"/>
-        <v>0.61477429397708572</v>
-      </c>
+        <f t="shared" si="12"/>
+        <v>0.61626143954403945</v>
+      </c>
+      <c r="I48" s="11"/>
+      <c r="J48" s="11"/>
       <c r="K48" s="11">
-        <f t="shared" si="25"/>
-        <v>90430.041071679705</v>
-      </c>
-    </row>
-    <row r="49" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
+        <f t="shared" si="11"/>
+        <v>89882.413179820607</v>
+      </c>
+      <c r="L48" s="11"/>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A49" s="4"/>
       <c r="B49" s="2"/>
-    </row>
-    <row r="50" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G49" s="3"/>
+      <c r="H49" s="3"/>
+      <c r="I49" s="3"/>
+      <c r="J49" s="3"/>
+      <c r="K49" s="3"/>
+      <c r="L49" s="3"/>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A50" s="6" t="s">
         <v>82</v>
       </c>
@@ -10277,22 +10382,28 @@
         <v>2835.9557466649489</v>
       </c>
       <c r="D50" s="3">
-        <v>3176.3845242761709</v>
+        <v>3168.719358388601</v>
+      </c>
+      <c r="E50" s="3">
+        <v>0</v>
       </c>
       <c r="G50" s="12">
-        <f t="shared" ref="G50:G52" si="29">C$63/C50</f>
+        <f t="shared" ref="G50:H52" si="14">C$63/C50</f>
         <v>-36.685392001385019</v>
       </c>
       <c r="H50" s="12">
-        <f t="shared" ref="H50:H52" si="30">D$63/D50</f>
-        <v>-43.921756621834106</v>
-      </c>
+        <f t="shared" si="14"/>
+        <v>-44.028003819045992</v>
+      </c>
+      <c r="I50" s="3"/>
+      <c r="J50" s="3"/>
       <c r="K50" s="3">
-        <f t="shared" si="25"/>
-        <v>-340.4287776112219</v>
-      </c>
-    </row>
-    <row r="51" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
+        <f t="shared" si="11"/>
+        <v>-332.76361172365205</v>
+      </c>
+      <c r="L50" s="3"/>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A51" s="10" t="s">
         <v>84</v>
       </c>
@@ -10303,22 +10414,28 @@
         <v>164074.67937628299</v>
       </c>
       <c r="D51" s="3">
-        <v>129300.9514225973</v>
+        <v>129856.2444803439</v>
+      </c>
+      <c r="E51" s="3">
+        <v>0</v>
       </c>
       <c r="G51" s="12">
-        <f t="shared" si="29"/>
+        <f t="shared" si="14"/>
         <v>-0.63409021221602901</v>
       </c>
       <c r="H51" s="12">
-        <f t="shared" si="30"/>
-        <v>-1.078974179831413</v>
-      </c>
+        <f t="shared" si="14"/>
+        <v>-1.0743602556112426</v>
+      </c>
+      <c r="I51" s="3"/>
+      <c r="J51" s="3"/>
       <c r="K51" s="3">
-        <f t="shared" si="25"/>
-        <v>34773.727953685695</v>
-      </c>
-    </row>
-    <row r="52" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.3">
+        <f t="shared" si="11"/>
+        <v>34218.434895939092</v>
+      </c>
+      <c r="L51" s="3"/>
+    </row>
+    <row r="52" spans="1:12" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A52" s="9" t="s">
         <v>105</v>
       </c>
@@ -10331,24 +10448,36 @@
       <c r="D52" s="11">
         <v>-359410.03202641761</v>
       </c>
+      <c r="E52" s="11">
+        <v>0</v>
+      </c>
       <c r="G52" s="14">
-        <f t="shared" si="29"/>
+        <f t="shared" si="14"/>
         <v>0.34289252201223486</v>
       </c>
       <c r="H52" s="14">
-        <f t="shared" si="30"/>
+        <f t="shared" si="14"/>
         <v>0.38817054500683429</v>
       </c>
+      <c r="I52" s="11"/>
+      <c r="J52" s="11"/>
       <c r="K52" s="11">
-        <f t="shared" si="25"/>
+        <f t="shared" si="11"/>
         <v>55996.741895605228</v>
       </c>
-    </row>
-    <row r="53" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="L52" s="11"/>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A53" s="5"/>
       <c r="B53" s="2"/>
-    </row>
-    <row r="54" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G53" s="3"/>
+      <c r="H53" s="3"/>
+      <c r="I53" s="3"/>
+      <c r="J53" s="3"/>
+      <c r="K53" s="3"/>
+      <c r="L53" s="3"/>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A54" s="6" t="s">
         <v>87</v>
       </c>
@@ -10361,20 +10490,26 @@
       <c r="D54" s="3">
         <v>14.381704120413239</v>
       </c>
+      <c r="E54" s="3">
+        <v>0</v>
+      </c>
       <c r="G54" s="12">
-        <f t="shared" ref="G54:G59" si="31">C$63/C54</f>
+        <f t="shared" ref="G54:H59" si="15">C$63/C54</f>
         <v>-397.47025053885034</v>
       </c>
       <c r="H54" s="12">
-        <f t="shared" ref="H54:H59" si="32">D$63/D54</f>
+        <f t="shared" si="15"/>
         <v>-9700.6854573371365</v>
       </c>
+      <c r="I54" s="3"/>
+      <c r="J54" s="3"/>
       <c r="K54" s="3">
-        <f t="shared" si="25"/>
+        <f t="shared" si="11"/>
         <v>247.36907628123868</v>
       </c>
-    </row>
-    <row r="55" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="L54" s="3"/>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A55" s="6" t="s">
         <v>89</v>
       </c>
@@ -10387,20 +10522,26 @@
       <c r="D55" s="3">
         <v>32114.197035891812</v>
       </c>
+      <c r="E55" s="3">
+        <v>0</v>
+      </c>
       <c r="G55" s="12">
-        <f t="shared" si="31"/>
+        <f t="shared" si="15"/>
         <v>-3.5713412956396322</v>
       </c>
       <c r="H55" s="12">
-        <f t="shared" si="32"/>
+        <f t="shared" si="15"/>
         <v>-4.3442589536551379</v>
       </c>
+      <c r="I55" s="3"/>
+      <c r="J55" s="3"/>
       <c r="K55" s="3">
-        <f t="shared" si="25"/>
+        <f t="shared" si="11"/>
         <v>-2982.8036314004021</v>
       </c>
-    </row>
-    <row r="56" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="L55" s="3"/>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A56" s="6" t="s">
         <v>91</v>
       </c>
@@ -10413,20 +10554,26 @@
       <c r="D56" s="3">
         <v>94407.704584843144</v>
       </c>
+      <c r="E56" s="3">
+        <v>0</v>
+      </c>
       <c r="G56" s="12">
-        <f t="shared" si="31"/>
+        <f t="shared" si="15"/>
         <v>-0.8617568312706656</v>
       </c>
       <c r="H56" s="12">
-        <f t="shared" si="32"/>
+        <f t="shared" si="15"/>
         <v>-1.477764856439657</v>
       </c>
+      <c r="I56" s="3"/>
+      <c r="J56" s="3"/>
       <c r="K56" s="3">
-        <f t="shared" si="25"/>
+        <f t="shared" si="11"/>
         <v>26320.260067992058</v>
       </c>
-    </row>
-    <row r="57" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="L56" s="3"/>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A57" s="6" t="s">
         <v>93</v>
       </c>
@@ -10439,20 +10586,26 @@
       <c r="D57" s="3">
         <v>416001.83584749012</v>
       </c>
+      <c r="E57" s="3">
+        <v>0</v>
+      </c>
       <c r="G57" s="12">
-        <f t="shared" si="31"/>
+        <f t="shared" si="15"/>
         <v>-0.22402937859407507</v>
       </c>
       <c r="H57" s="12">
-        <f t="shared" si="32"/>
+        <f t="shared" si="15"/>
         <v>-0.33536483734116196</v>
       </c>
+      <c r="I57" s="3"/>
+      <c r="J57" s="3"/>
       <c r="K57" s="3">
-        <f t="shared" si="25"/>
+        <f t="shared" si="11"/>
         <v>48393.275712827803</v>
       </c>
-    </row>
-    <row r="58" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="L57" s="3"/>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A58" s="6" t="s">
         <v>95</v>
       </c>
@@ -10465,20 +10618,26 @@
       <c r="D58" s="3">
         <v>130448.5642588777</v>
       </c>
+      <c r="E58" s="3">
+        <v>0</v>
+      </c>
       <c r="G58" s="12">
-        <f t="shared" si="31"/>
+        <f t="shared" si="15"/>
         <v>-0.6125947645635097</v>
       </c>
       <c r="H58" s="12">
-        <f t="shared" si="32"/>
+        <f t="shared" si="15"/>
         <v>-1.0694819740273511</v>
       </c>
+      <c r="I58" s="3"/>
+      <c r="J58" s="3"/>
       <c r="K58" s="3">
-        <f t="shared" si="25"/>
+        <f t="shared" si="11"/>
         <v>39383.36099290631</v>
       </c>
-    </row>
-    <row r="59" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="L58" s="3"/>
+    </row>
+    <row r="59" spans="1:12" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A59" s="4" t="s">
         <v>97</v>
       </c>
@@ -10491,24 +10650,36 @@
       <c r="D59" s="11">
         <v>-136135.8862826362</v>
       </c>
+      <c r="E59" s="11">
+        <v>0</v>
+      </c>
       <c r="G59" s="14">
-        <f t="shared" si="31"/>
+        <f t="shared" si="15"/>
         <v>1.0384611158022257</v>
       </c>
       <c r="H59" s="14">
-        <f t="shared" si="32"/>
+        <f t="shared" si="15"/>
         <v>1.0248024369046382</v>
       </c>
+      <c r="I59" s="11"/>
+      <c r="J59" s="11"/>
       <c r="K59" s="11">
-        <f t="shared" si="25"/>
+        <f t="shared" si="11"/>
         <v>35950.961992415396</v>
       </c>
-    </row>
-    <row r="60" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="L59" s="11"/>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A60" s="4"/>
       <c r="B60" s="2"/>
-    </row>
-    <row r="61" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G60" s="3"/>
+      <c r="H60" s="3"/>
+      <c r="I60" s="3"/>
+      <c r="J60" s="3"/>
+      <c r="K60" s="3"/>
+      <c r="L60" s="3"/>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A61" s="6" t="s">
         <v>99</v>
       </c>
@@ -10521,20 +10692,26 @@
       <c r="D61" s="3">
         <v>-2097.7035648956862</v>
       </c>
+      <c r="E61" s="3">
+        <v>0</v>
+      </c>
       <c r="G61" s="12">
-        <f t="shared" ref="G61:G63" si="33">C$63/C61</f>
+        <f t="shared" ref="G61:H63" si="16">C$63/C61</f>
         <v>214.47258621474552</v>
       </c>
       <c r="H61" s="12">
-        <f t="shared" ref="H61:H63" si="34">D$63/D61</f>
+        <f t="shared" si="16"/>
         <v>66.507198799347947</v>
       </c>
+      <c r="I61" s="3"/>
+      <c r="J61" s="3"/>
       <c r="K61" s="3">
-        <f t="shared" si="25"/>
+        <f t="shared" si="11"/>
         <v>1612.6152368199776</v>
       </c>
-    </row>
-    <row r="62" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="L61" s="3"/>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A62" s="6" t="s">
         <v>101</v>
       </c>
@@ -10547,20 +10724,26 @@
       <c r="D62" s="3">
         <v>-1278.7981650864219</v>
       </c>
+      <c r="E62" s="3">
+        <v>0</v>
+      </c>
       <c r="G62" s="12">
-        <f t="shared" si="33"/>
+        <f t="shared" si="16"/>
         <v>30.888942482853313</v>
       </c>
       <c r="H62" s="12">
-        <f t="shared" si="34"/>
+        <f t="shared" si="16"/>
         <v>109.09648748455153</v>
       </c>
+      <c r="I62" s="3"/>
+      <c r="J62" s="3"/>
       <c r="K62" s="3">
-        <f t="shared" si="25"/>
+        <f t="shared" si="11"/>
         <v>-2089.3374816012738</v>
       </c>
-    </row>
-    <row r="63" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="L62" s="3"/>
+    </row>
+    <row r="63" spans="1:12" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A63" s="4" t="s">
         <v>103</v>
       </c>
@@ -10573,170 +10756,176 @@
       <c r="D63" s="11">
         <v>-139512.38801261829</v>
       </c>
+      <c r="E63" s="11">
+        <v>0</v>
+      </c>
       <c r="G63" s="14">
-        <f t="shared" si="33"/>
+        <f t="shared" si="16"/>
         <v>1</v>
       </c>
       <c r="H63" s="14">
-        <f t="shared" si="34"/>
+        <f t="shared" si="16"/>
         <v>1</v>
       </c>
+      <c r="I63" s="11"/>
+      <c r="J63" s="11"/>
       <c r="K63" s="11">
-        <f t="shared" si="25"/>
+        <f t="shared" si="11"/>
         <v>35474.239747634099</v>
       </c>
+      <c r="L63" s="11"/>
     </row>
     <row r="66" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C66" s="15">
+      <c r="C66" s="3">
         <f>SUM(C3:C11)-C12</f>
         <v>0</v>
       </c>
-      <c r="D66" s="15">
-        <f t="shared" ref="D66:E66" si="35">SUM(D3:D11)-D12</f>
-        <v>0</v>
-      </c>
-      <c r="E66" s="15">
-        <f t="shared" si="35"/>
+      <c r="D66" s="3">
+        <f t="shared" ref="D66:E66" si="17">SUM(D3:D11)-D12</f>
+        <v>0</v>
+      </c>
+      <c r="E66" s="3">
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
     <row r="67" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C67" s="15">
+      <c r="C67" s="3">
         <f>SUM(C14:C19)-C20</f>
         <v>0</v>
       </c>
-      <c r="D67" s="15">
-        <f t="shared" ref="D67:E67" si="36">SUM(D14:D19)-D20</f>
-        <v>0</v>
-      </c>
-      <c r="E67" s="15">
-        <f t="shared" si="36"/>
+      <c r="D67" s="3">
+        <f t="shared" ref="D67:E67" si="18">SUM(D14:D19)-D20</f>
+        <v>0</v>
+      </c>
+      <c r="E67" s="3">
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
     </row>
     <row r="68" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C68" s="15">
+      <c r="C68" s="3">
         <f>SUM(C22:C27)-C28</f>
         <v>0</v>
       </c>
-      <c r="D68" s="15">
-        <f t="shared" ref="D68:E68" si="37">SUM(D22:D27)-D28</f>
-        <v>0</v>
-      </c>
-      <c r="E68" s="15">
-        <f t="shared" si="37"/>
+      <c r="D68" s="3">
+        <f t="shared" ref="D68:E68" si="19">SUM(D22:D27)-D28</f>
+        <v>0</v>
+      </c>
+      <c r="E68" s="3">
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
     <row r="69" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C69" s="15">
+      <c r="C69" s="3">
         <f>SUM(C30:C33)-C34</f>
         <v>0</v>
       </c>
-      <c r="D69" s="15">
-        <f t="shared" ref="D69:E69" si="38">SUM(D30:D33)-D34</f>
-        <v>0</v>
-      </c>
-      <c r="E69" s="15">
-        <f t="shared" si="38"/>
+      <c r="D69" s="3">
+        <f t="shared" ref="D69:E69" si="20">SUM(D30:D33)-D34</f>
+        <v>0</v>
+      </c>
+      <c r="E69" s="3">
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
     </row>
     <row r="70" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C70" s="15">
+      <c r="C70" s="3">
         <f>SUM(C36:C40)-C41</f>
         <v>0</v>
       </c>
-      <c r="D70" s="15">
-        <f t="shared" ref="D70:E70" si="39">SUM(D36:D40)-D41</f>
-        <v>0</v>
-      </c>
-      <c r="E70" s="15">
-        <f t="shared" si="39"/>
+      <c r="D70" s="3">
+        <f t="shared" ref="D70:E70" si="21">SUM(D36:D40)-D41</f>
+        <v>0</v>
+      </c>
+      <c r="E70" s="3">
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
     <row r="71" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C71" s="15">
+      <c r="C71" s="3">
         <f>SUM(C12,C20)-C43</f>
         <v>0</v>
       </c>
-      <c r="D71" s="15">
-        <f t="shared" ref="D71:E71" si="40">SUM(D12,D20)-D43</f>
-        <v>0</v>
-      </c>
-      <c r="E71" s="15">
-        <f t="shared" si="40"/>
+      <c r="D71" s="3">
+        <f t="shared" ref="D71:E71" si="22">SUM(D12,D20)-D43</f>
+        <v>0</v>
+      </c>
+      <c r="E71" s="3">
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
     </row>
     <row r="72" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C72" s="15">
+      <c r="C72" s="3">
         <f>SUM(C28,C34,C41)-C44</f>
         <v>0</v>
       </c>
-      <c r="D72" s="15">
-        <f t="shared" ref="D72:E72" si="41">SUM(D28,D34,D41)-D44</f>
-        <v>0</v>
-      </c>
-      <c r="E72" s="15">
-        <f t="shared" si="41"/>
+      <c r="D72" s="3">
+        <f t="shared" ref="D72:E72" si="23">SUM(D28,D34,D41)-D44</f>
+        <v>0</v>
+      </c>
+      <c r="E72" s="3">
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
     </row>
     <row r="73" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C73" s="15">
+      <c r="C73" s="3">
         <f>C46-C47-C48</f>
         <v>5.2386894822120667E-10</v>
       </c>
-      <c r="D73" s="15">
-        <f t="shared" ref="D73:E73" si="42">D46-D47-D48</f>
-        <v>3.2014213502407074E-10</v>
-      </c>
-      <c r="E73" s="15">
-        <f t="shared" si="42"/>
+      <c r="D73" s="3">
+        <f t="shared" ref="D73:E73" si="24">D46-D47-D48</f>
+        <v>2.6193447411060333E-10</v>
+      </c>
+      <c r="E73" s="3">
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
     </row>
     <row r="74" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C74" s="15">
+      <c r="C74" s="3">
         <f>C48-C50-C51-C52</f>
         <v>0</v>
       </c>
-      <c r="D74" s="15">
-        <f t="shared" ref="D74:E74" si="43">D48-D50-D51-D52</f>
-        <v>0</v>
-      </c>
-      <c r="E74" s="15">
-        <f t="shared" si="43"/>
+      <c r="D74" s="3">
+        <f t="shared" ref="D74:E74" si="25">D48-D50-D51-D52</f>
+        <v>0</v>
+      </c>
+      <c r="E74" s="3">
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
     </row>
     <row r="75" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C75" s="15">
+      <c r="C75" s="3">
         <f>C52+C54+C55-C56+C57-C58-C59</f>
         <v>1.7462298274040222E-10</v>
       </c>
-      <c r="D75" s="15">
-        <f t="shared" ref="D75:E75" si="44">D52+D54+D55-D56+D57-D58-D59</f>
-        <v>0</v>
-      </c>
-      <c r="E75" s="15">
-        <f t="shared" si="44"/>
+      <c r="D75" s="3">
+        <f t="shared" ref="D75:E75" si="26">D52+D54+D55-D56+D57-D58-D59</f>
+        <v>0</v>
+      </c>
+      <c r="E75" s="3">
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
     </row>
     <row r="76" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C76" s="15">
+      <c r="C76" s="3">
         <f>C59+C61+C62-C63</f>
         <v>0</v>
       </c>
-      <c r="D76" s="15">
-        <f t="shared" ref="D76:E76" si="45">D59+D61+D62-D63</f>
-        <v>0</v>
-      </c>
-      <c r="E76" s="15">
-        <f t="shared" si="45"/>
+      <c r="D76" s="3">
+        <f t="shared" ref="D76:E76" si="27">D59+D61+D62-D63</f>
+        <v>0</v>
+      </c>
+      <c r="E76" s="3">
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
     </row>
@@ -14712,17 +14901,18 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:L76"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB56CAE3-BA6F-45F6-A919-4E6C03DC2D39}">
+  <dimension ref="A1:L63"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="58.33203125" customWidth="1"/>
     <col min="2" max="2" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="12.6640625" style="3" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8.5546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.21875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10.21875" bestFit="1" customWidth="1"/>
@@ -14740,13 +14930,13 @@
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="G2" s="1" t="s">
@@ -14765,7 +14955,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="3" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>5</v>
       </c>
@@ -14776,33 +14966,34 @@
         <v>94.20405209251976</v>
       </c>
       <c r="D3" s="3">
-        <v>214.39122198970711</v>
+        <v>188.68909659694381</v>
       </c>
       <c r="E3" s="3">
-        <v>462.95221418137578</v>
+        <v>460.16492014099242</v>
       </c>
       <c r="G3" s="12">
         <f>C3/C$43</f>
         <v>1.5101970723879868E-5</v>
       </c>
       <c r="H3" s="12">
-        <f t="shared" ref="H3:H12" si="0">D3/D$43</f>
-        <v>4.1342674471796046E-6</v>
+        <f t="shared" ref="H3:I12" si="0">D3/D$43</f>
+        <v>3.5092424289125801E-5</v>
       </c>
       <c r="I3" s="12">
-        <f t="shared" ref="I3:I12" si="1">E3/E$43</f>
-        <v>8.4522371443225266E-6</v>
-      </c>
+        <f t="shared" si="0"/>
+        <v>8.102855891440438E-5</v>
+      </c>
+      <c r="J3" s="3"/>
       <c r="K3" s="3">
         <f>C3-D3</f>
-        <v>-120.18716989718735</v>
+        <v>-94.485044504424053</v>
       </c>
       <c r="L3" s="3">
         <f>D3-E3</f>
-        <v>-248.56099219166867</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+        <v>-271.47582354404858</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>7</v>
       </c>
@@ -14813,33 +15004,34 @@
         <v>7.4528522225094748E-2</v>
       </c>
       <c r="D4" s="3">
-        <v>7.4385766143540921E-2</v>
+        <v>6.7405011882690061E-2</v>
       </c>
       <c r="E4" s="3">
-        <v>7.4507939144015906E-2</v>
+        <v>7.1210913051840338E-2</v>
       </c>
       <c r="G4" s="12">
-        <f t="shared" ref="G4:G12" si="2">C4/C$43</f>
+        <f t="shared" ref="G4:G12" si="1">C4/C$43</f>
         <v>1.1947761648639135E-8</v>
       </c>
       <c r="H4" s="12">
         <f t="shared" si="0"/>
-        <v>1.4344367677307261E-9</v>
+        <v>1.2535993435029455E-8</v>
       </c>
       <c r="I4" s="12">
-        <f t="shared" si="1"/>
-        <v>1.3603105277151697E-9</v>
-      </c>
+        <f t="shared" si="0"/>
+        <v>1.2539238457815591E-8</v>
+      </c>
+      <c r="J4" s="3"/>
       <c r="K4" s="3">
-        <f t="shared" ref="K4:K12" si="3">C4-D4</f>
-        <v>1.4275608155382702E-4</v>
+        <f t="shared" ref="K4:L12" si="2">C4-D4</f>
+        <v>7.1235103424046875E-3</v>
       </c>
       <c r="L4" s="3">
-        <f t="shared" ref="L4:L12" si="4">D4-E4</f>
-        <v>-1.2217300047498436E-4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+        <f t="shared" si="2"/>
+        <v>-3.8059011691502775E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>9</v>
       </c>
@@ -14850,33 +15042,34 @@
         <v>7.4528522225094748E-2</v>
       </c>
       <c r="D5" s="3">
-        <v>7.4385766143540921E-2</v>
+        <v>6.7405011882690061E-2</v>
       </c>
       <c r="E5" s="3">
-        <v>7.4507939144015906E-2</v>
+        <v>7.1210913051840338E-2</v>
       </c>
       <c r="G5" s="12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1.1947761648639135E-8</v>
       </c>
       <c r="H5" s="12">
         <f t="shared" si="0"/>
-        <v>1.4344367677307261E-9</v>
+        <v>1.2535993435029455E-8</v>
       </c>
       <c r="I5" s="12">
-        <f t="shared" si="1"/>
-        <v>1.3603105277151697E-9</v>
-      </c>
+        <f t="shared" si="0"/>
+        <v>1.2539238457815591E-8</v>
+      </c>
+      <c r="J5" s="3"/>
       <c r="K5" s="3">
-        <f t="shared" si="3"/>
-        <v>1.4275608155382702E-4</v>
+        <f t="shared" si="2"/>
+        <v>7.1235103424046875E-3</v>
       </c>
       <c r="L5" s="3">
-        <f t="shared" si="4"/>
-        <v>-1.2217300047498436E-4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+        <f t="shared" si="2"/>
+        <v>-3.8059011691502775E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>11</v>
       </c>
@@ -14887,33 +15080,34 @@
         <v>7.4528522225094748E-2</v>
       </c>
       <c r="D6" s="3">
-        <v>7.4385766143540921E-2</v>
+        <v>6.7405011882690061E-2</v>
       </c>
       <c r="E6" s="3">
-        <v>7.4507939144015906E-2</v>
+        <v>7.1210913051840338E-2</v>
       </c>
       <c r="G6" s="12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1.1947761648639135E-8</v>
       </c>
       <c r="H6" s="12">
         <f t="shared" si="0"/>
-        <v>1.4344367677307261E-9</v>
+        <v>1.2535993435029455E-8</v>
       </c>
       <c r="I6" s="12">
-        <f t="shared" si="1"/>
-        <v>1.3603105277151697E-9</v>
-      </c>
+        <f t="shared" si="0"/>
+        <v>1.2539238457815591E-8</v>
+      </c>
+      <c r="J6" s="3"/>
       <c r="K6" s="3">
-        <f t="shared" si="3"/>
-        <v>1.4275608155382702E-4</v>
+        <f t="shared" si="2"/>
+        <v>7.1235103424046875E-3</v>
       </c>
       <c r="L6" s="3">
-        <f t="shared" si="4"/>
-        <v>-1.2217300047498436E-4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+        <f t="shared" si="2"/>
+        <v>-3.8059011691502775E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>13</v>
       </c>
@@ -14924,33 +15118,34 @@
         <v>1295983.0314821289</v>
       </c>
       <c r="D7" s="3">
-        <v>791248.8044355493</v>
+        <v>749959.05935039767</v>
       </c>
       <c r="E7" s="3">
-        <v>764039.98265799053</v>
+        <v>761783.88142628723</v>
       </c>
       <c r="G7" s="12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0.20776067871121109</v>
       </c>
       <c r="H7" s="12">
         <f t="shared" si="0"/>
-        <v>1.5258246790322061E-2</v>
+        <v>0.13947748961040976</v>
       </c>
       <c r="I7" s="12">
-        <f t="shared" si="1"/>
-        <v>1.3949273647148701E-2</v>
-      </c>
+        <f t="shared" si="0"/>
+        <v>0.13413940831752433</v>
+      </c>
+      <c r="J7" s="3"/>
       <c r="K7" s="3">
-        <f t="shared" si="3"/>
-        <v>504734.22704657959</v>
+        <f t="shared" si="2"/>
+        <v>546023.97213173122</v>
       </c>
       <c r="L7" s="3">
-        <f t="shared" si="4"/>
-        <v>27208.821777558769</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+        <f t="shared" si="2"/>
+        <v>-11824.822075889562</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>15</v>
       </c>
@@ -14961,33 +15156,34 @@
         <v>3402.5003108237338</v>
       </c>
       <c r="D8" s="3">
-        <v>5570.8415782019574</v>
+        <v>3077.285944155039</v>
       </c>
       <c r="E8" s="3">
-        <v>5579.9912645742979</v>
+        <v>3251.0392874977019</v>
       </c>
       <c r="G8" s="12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>5.4545912771975489E-4</v>
       </c>
       <c r="H8" s="12">
         <f t="shared" si="0"/>
-        <v>1.074267349959913E-4</v>
+        <v>5.7231406561835654E-4</v>
       </c>
       <c r="I8" s="12">
-        <f t="shared" si="1"/>
-        <v>1.0187532964893087E-4</v>
-      </c>
+        <f t="shared" si="0"/>
+        <v>5.7246221280696046E-4</v>
+      </c>
+      <c r="J8" s="3"/>
       <c r="K8" s="3">
-        <f t="shared" si="3"/>
-        <v>-2168.3412673782236</v>
+        <f t="shared" si="2"/>
+        <v>325.21436666869477</v>
       </c>
       <c r="L8" s="3">
-        <f t="shared" si="4"/>
-        <v>-9.1496863723405113</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+        <f t="shared" si="2"/>
+        <v>-173.7533433426629</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>17</v>
       </c>
@@ -14998,33 +15194,34 @@
         <v>1.229720616714064</v>
       </c>
       <c r="D9" s="3">
-        <v>46284039.615688533</v>
+        <v>27915.785671216101</v>
       </c>
       <c r="E9" s="3">
-        <v>48966898.443064027</v>
+        <v>1.1749800653553659</v>
       </c>
       <c r="G9" s="12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1.9713806720254583E-7</v>
       </c>
       <c r="H9" s="12">
         <f t="shared" si="0"/>
-        <v>0.89253000440614616</v>
+        <v>5.191781681117451E-3</v>
       </c>
       <c r="I9" s="12">
-        <f t="shared" si="1"/>
-        <v>0.89400120613870626</v>
-      </c>
+        <f t="shared" si="0"/>
+        <v>2.0689743455395731E-7</v>
+      </c>
+      <c r="J9" s="3"/>
       <c r="K9" s="3">
-        <f t="shared" si="3"/>
-        <v>-46284038.385967918</v>
+        <f t="shared" si="2"/>
+        <v>-27914.555950599388</v>
       </c>
       <c r="L9" s="3">
-        <f t="shared" si="4"/>
-        <v>-2682858.8273754939</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+        <f t="shared" si="2"/>
+        <v>27914.610691150745</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
         <v>19</v>
       </c>
@@ -15035,33 +15232,34 @@
         <v>180256.47253814759</v>
       </c>
       <c r="D10" s="3">
-        <v>31699.53429594405</v>
+        <v>30045.357148300511</v>
       </c>
       <c r="E10" s="3">
-        <v>30379.053250630401</v>
+        <v>30289.348233861139</v>
       </c>
       <c r="G10" s="12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>2.8897143069678183E-2</v>
       </c>
       <c r="H10" s="12">
         <f t="shared" si="0"/>
-        <v>6.1128600095747786E-4</v>
+        <v>5.5878396790392916E-3</v>
       </c>
       <c r="I10" s="12">
-        <f t="shared" si="1"/>
-        <v>5.5463815579404985E-4</v>
-      </c>
+        <f t="shared" si="0"/>
+        <v>5.33352746031649E-3</v>
+      </c>
+      <c r="J10" s="3"/>
       <c r="K10" s="3">
-        <f t="shared" si="3"/>
-        <v>148556.93824220353</v>
+        <f t="shared" si="2"/>
+        <v>150211.11538984708</v>
       </c>
       <c r="L10" s="3">
-        <f t="shared" si="4"/>
-        <v>1320.4810453136488</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+        <f t="shared" si="2"/>
+        <v>-243.99108556062856</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
         <v>21</v>
       </c>
@@ -15072,33 +15270,34 @@
         <v>7.4528522225094748E-2</v>
       </c>
       <c r="D11" s="3">
-        <v>30442.477789920329</v>
+        <v>28585.07250253663</v>
       </c>
       <c r="E11" s="3">
-        <v>26415.88999686118</v>
+        <v>26161.71447518079</v>
       </c>
       <c r="G11" s="12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1.1947761648639135E-8</v>
       </c>
       <c r="H11" s="12">
         <f t="shared" si="0"/>
-        <v>5.8704523333701661E-4</v>
+        <v>5.3162557385983376E-3</v>
       </c>
       <c r="I11" s="12">
-        <f t="shared" si="1"/>
-        <v>4.822816692358095E-4</v>
-      </c>
+        <f t="shared" si="0"/>
+        <v>4.6067093119668955E-3</v>
+      </c>
+      <c r="J11" s="3"/>
       <c r="K11" s="3">
-        <f t="shared" si="3"/>
-        <v>-30442.403261398103</v>
+        <f t="shared" si="2"/>
+        <v>-28584.997974014404</v>
       </c>
       <c r="L11" s="3">
-        <f t="shared" si="4"/>
-        <v>4026.5877930591487</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.3">
+        <f t="shared" si="2"/>
+        <v>2423.35802735584</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>23</v>
       </c>
@@ -15109,37 +15308,44 @@
         <v>1479737.7362178981</v>
       </c>
       <c r="D12" s="11">
-        <v>47143215.888167433</v>
+        <v>839771.4519282385</v>
       </c>
       <c r="E12" s="11">
-        <v>49793776.535972089</v>
+        <v>821947.53695577243</v>
       </c>
       <c r="G12" s="13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0.23721862780844666</v>
       </c>
       <c r="H12" s="13">
         <f t="shared" si="0"/>
-        <v>0.90909814773651609</v>
+        <v>0.15618081080705262</v>
       </c>
       <c r="I12" s="13">
-        <f t="shared" si="1"/>
-        <v>0.90909773125860982</v>
-      </c>
+        <f t="shared" si="0"/>
+        <v>0.14473338037667902</v>
+      </c>
+      <c r="J12" s="11"/>
       <c r="K12" s="11">
-        <f t="shared" si="3"/>
-        <v>-45663478.151949532</v>
+        <f t="shared" si="2"/>
+        <v>639966.28428965958</v>
       </c>
       <c r="L12" s="11">
-        <f t="shared" si="4"/>
-        <v>-2650560.6478046551</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+        <f t="shared" si="2"/>
+        <v>17823.914972466067</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="4"/>
       <c r="B13" s="2"/>
-    </row>
-    <row r="14" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
         <v>25</v>
       </c>
@@ -15150,33 +15356,34 @@
         <v>16906.16354694113</v>
       </c>
       <c r="D14" s="3">
-        <v>13161.574475330681</v>
+        <v>12780.83526541502</v>
       </c>
       <c r="E14" s="3">
-        <v>21108.744420045019</v>
+        <v>20659.92483858551</v>
       </c>
       <c r="G14" s="12">
-        <f t="shared" ref="G14:G20" si="5">C14/C$43</f>
+        <f t="shared" ref="G14:I20" si="3">C14/C$43</f>
         <v>2.7102484581902953E-3</v>
       </c>
       <c r="H14" s="12">
-        <f t="shared" ref="H14:H20" si="6">D14/D$43</f>
-        <v>2.5380455599810893E-4</v>
+        <f t="shared" si="3"/>
+        <v>2.3769815108152371E-3</v>
       </c>
       <c r="I14" s="12">
-        <f t="shared" ref="I14:I20" si="7">E14/E$43</f>
-        <v>3.8538775318874564E-4</v>
-      </c>
+        <f t="shared" si="3"/>
+        <v>3.6379216747716731E-3</v>
+      </c>
+      <c r="J14" s="3"/>
       <c r="K14" s="3">
-        <f t="shared" ref="K14:K20" si="8">C14-D14</f>
-        <v>3744.5890716104495</v>
+        <f t="shared" ref="K14:L20" si="4">C14-D14</f>
+        <v>4125.32828152611</v>
       </c>
       <c r="L14" s="3">
-        <f t="shared" ref="L14:L20" si="9">D14-E14</f>
-        <v>-7947.1699447143383</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+        <f t="shared" si="4"/>
+        <v>-7879.0895731704895</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
         <v>27</v>
       </c>
@@ -15187,33 +15394,34 @@
         <v>5136.0403720191553</v>
       </c>
       <c r="D15" s="3">
-        <v>1108.2012918326441</v>
+        <v>375.94864528082809</v>
       </c>
       <c r="E15" s="3">
-        <v>26379.74695823573</v>
+        <v>25725.3073856962</v>
       </c>
       <c r="G15" s="12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>8.233651272104601E-4</v>
       </c>
       <c r="H15" s="12">
-        <f t="shared" si="6"/>
-        <v>2.1370280383802503E-5</v>
+        <f t="shared" si="3"/>
+        <v>6.9918981059611252E-5</v>
       </c>
       <c r="I15" s="12">
-        <f t="shared" si="7"/>
-        <v>4.8162179652277173E-4</v>
-      </c>
+        <f t="shared" si="3"/>
+        <v>4.5298641722936427E-3</v>
+      </c>
+      <c r="J15" s="3"/>
       <c r="K15" s="3">
-        <f t="shared" si="8"/>
-        <v>4027.8390801865112</v>
+        <f t="shared" si="4"/>
+        <v>4760.0917267383275</v>
       </c>
       <c r="L15" s="3">
-        <f t="shared" si="9"/>
-        <v>-25271.545666403086</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+        <f t="shared" si="4"/>
+        <v>-25349.358740415373</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
         <v>29</v>
       </c>
@@ -15224,33 +15432,34 @@
         <v>4519681.9287171513</v>
       </c>
       <c r="D16" s="3">
-        <v>4527677.8621861665</v>
+        <v>4355737.7390213041</v>
       </c>
       <c r="E16" s="3">
-        <v>4835718.4881302398</v>
+        <v>4715752.0022763861</v>
       </c>
       <c r="G16" s="12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>0.72455592570157779</v>
       </c>
       <c r="H16" s="12">
-        <f t="shared" si="6"/>
-        <v>8.7310623183306887E-2</v>
+        <f t="shared" si="3"/>
+        <v>0.8100807072938675</v>
       </c>
       <c r="I16" s="12">
-        <f t="shared" si="7"/>
-        <v>8.8286950948350942E-2</v>
-      </c>
+        <f t="shared" si="3"/>
+        <v>0.83037748471807815</v>
+      </c>
+      <c r="J16" s="3"/>
       <c r="K16" s="3">
-        <f t="shared" si="8"/>
-        <v>-7995.9334690151736</v>
+        <f t="shared" si="4"/>
+        <v>163944.18969584722</v>
       </c>
       <c r="L16" s="3">
-        <f t="shared" si="9"/>
-        <v>-308040.62594407331</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+        <f t="shared" si="4"/>
+        <v>-360014.26325508207</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" s="6" t="s">
         <v>31</v>
       </c>
@@ -15261,33 +15470,34 @@
         <v>16536.56661182045</v>
       </c>
       <c r="D17" s="3">
-        <v>6649.7786915905936</v>
+        <v>6485.3674657609154</v>
       </c>
       <c r="E17" s="3">
-        <v>3814.284375623306</v>
+        <v>3719.6580457999339</v>
       </c>
       <c r="G17" s="12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>2.6509979061190704E-3</v>
       </c>
       <c r="H17" s="12">
-        <f t="shared" si="6"/>
-        <v>1.2823269218042641E-4</v>
+        <f t="shared" si="3"/>
+        <v>1.2061495384946416E-3</v>
       </c>
       <c r="I17" s="12">
-        <f t="shared" si="7"/>
-        <v>6.963836674949274E-5</v>
-      </c>
+        <f t="shared" si="3"/>
+        <v>6.5497937351067766E-4</v>
+      </c>
+      <c r="J17" s="3"/>
       <c r="K17" s="3">
-        <f t="shared" si="8"/>
-        <v>9886.7879202298573</v>
+        <f t="shared" si="4"/>
+        <v>10051.199146059535</v>
       </c>
       <c r="L17" s="3">
-        <f t="shared" si="9"/>
-        <v>2835.4943159672875</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+        <f t="shared" si="4"/>
+        <v>2765.7094199609814</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
         <v>33</v>
       </c>
@@ -15298,33 +15508,34 @@
         <v>198830.48006754721</v>
       </c>
       <c r="D18" s="3">
-        <v>165068.58155017241</v>
+        <v>161531.25013744039</v>
       </c>
       <c r="E18" s="3">
-        <v>64133.725016675598</v>
+        <v>63864.924450082137</v>
       </c>
       <c r="G18" s="12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>3.1874765705895876E-2</v>
       </c>
       <c r="H18" s="12">
-        <f t="shared" si="6"/>
-        <v>3.1831418139300193E-3</v>
+        <f t="shared" si="3"/>
+        <v>3.0041604247459108E-2</v>
       </c>
       <c r="I18" s="12">
-        <f t="shared" si="7"/>
-        <v>1.1709058433779049E-3</v>
-      </c>
+        <f t="shared" si="3"/>
+        <v>1.1245713366811847E-2</v>
+      </c>
+      <c r="J18" s="3"/>
       <c r="K18" s="3">
-        <f t="shared" si="8"/>
-        <v>33761.898517374793</v>
+        <f t="shared" si="4"/>
+        <v>37299.229930106812</v>
       </c>
       <c r="L18" s="3">
-        <f t="shared" si="9"/>
-        <v>100934.85653349682</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+        <f t="shared" si="4"/>
+        <v>97666.325687358258</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" s="6" t="s">
         <v>35</v>
       </c>
@@ -15335,33 +15546,34 @@
         <v>1035.91779995404</v>
       </c>
       <c r="D19" s="3">
-        <v>242.6777400453789</v>
+        <v>235.65753655968049</v>
       </c>
       <c r="E19" s="3">
-        <v>27811.628973243802</v>
+        <v>27376.7293810099</v>
       </c>
       <c r="G19" s="12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>1.6606929255959458E-4</v>
       </c>
       <c r="H19" s="12">
-        <f t="shared" si="6"/>
-        <v>4.6797376847494829E-6</v>
+        <f t="shared" si="3"/>
+        <v>4.3827621251202858E-5</v>
       </c>
       <c r="I19" s="12">
-        <f t="shared" si="7"/>
-        <v>5.0776403320035041E-4</v>
-      </c>
+        <f t="shared" si="3"/>
+        <v>4.8206563178548904E-3</v>
+      </c>
+      <c r="J19" s="3"/>
       <c r="K19" s="3">
-        <f t="shared" si="8"/>
-        <v>793.24005990866112</v>
+        <f t="shared" si="4"/>
+        <v>800.26026339435953</v>
       </c>
       <c r="L19" s="3">
-        <f t="shared" si="9"/>
-        <v>-27568.951233198422</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.3">
+        <f t="shared" si="4"/>
+        <v>-27141.07184445022</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
         <v>37</v>
       </c>
@@ -15372,37 +15584,44 @@
         <v>4758127.0971154347</v>
       </c>
       <c r="D20" s="11">
-        <v>4713908.675935138</v>
+        <v>4537146.7980717607</v>
       </c>
       <c r="E20" s="11">
-        <v>4978966.6178740636</v>
+        <v>4857098.5463775601</v>
       </c>
       <c r="G20" s="13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>0.76278137219155329</v>
       </c>
       <c r="H20" s="13">
-        <f t="shared" si="6"/>
-        <v>9.090185226348399E-2</v>
+        <f t="shared" si="3"/>
+        <v>0.84381918919294718</v>
       </c>
       <c r="I20" s="13">
-        <f t="shared" si="7"/>
-        <v>9.0902268741390208E-2</v>
-      </c>
+        <f t="shared" si="3"/>
+        <v>0.85526661962332096</v>
+      </c>
+      <c r="J20" s="11"/>
       <c r="K20" s="11">
-        <f t="shared" si="8"/>
-        <v>44218.421180296689</v>
+        <f t="shared" si="4"/>
+        <v>220980.29904367402</v>
       </c>
       <c r="L20" s="11">
-        <f t="shared" si="9"/>
-        <v>-265057.94193892553</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+        <f t="shared" si="4"/>
+        <v>-319951.74830579944</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" s="4"/>
       <c r="B21" s="2"/>
-    </row>
-    <row r="22" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="3"/>
+      <c r="L21" s="3"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" s="6" t="s">
         <v>39</v>
       </c>
@@ -15413,33 +15632,34 @@
         <v>415025.4380640529</v>
       </c>
       <c r="D22" s="3">
-        <v>308172.0146836245</v>
+        <v>294859.51443682268</v>
       </c>
       <c r="E22" s="3">
-        <v>423166.94889196247</v>
+        <v>383262.74624740798</v>
       </c>
       <c r="G22" s="12">
-        <f t="shared" ref="G22:G28" si="10">C22/C$43</f>
+        <f t="shared" ref="G22:I28" si="5">C22/C$43</f>
         <v>6.6533252828159695E-2</v>
       </c>
       <c r="H22" s="12">
-        <f t="shared" ref="H22:H28" si="11">D22/D$43</f>
-        <v>5.9427131232986383E-3</v>
+        <f t="shared" si="5"/>
+        <v>5.4838013287039036E-2</v>
       </c>
       <c r="I22" s="12">
-        <f t="shared" ref="I22:I28" si="12">E22/E$43</f>
-        <v>7.725867366243964E-3</v>
-      </c>
+        <f t="shared" si="5"/>
+        <v>6.748716960973325E-2</v>
+      </c>
+      <c r="J22" s="3"/>
       <c r="K22" s="3">
-        <f t="shared" ref="K22:K28" si="13">C22-D22</f>
-        <v>106853.4233804284</v>
+        <f t="shared" ref="K22:L28" si="6">C22-D22</f>
+        <v>120165.92362723022</v>
       </c>
       <c r="L22" s="3">
-        <f t="shared" ref="L22:L28" si="14">D22-E22</f>
-        <v>-114994.93420833797</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+        <f t="shared" si="6"/>
+        <v>-88403.231810585305</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
         <v>41</v>
       </c>
@@ -15450,33 +15670,34 @@
         <v>5.299540684366523E-2</v>
       </c>
       <c r="D23" s="3">
-        <v>4.0776848963182177E-2</v>
+        <v>3.7651185918134829E-2</v>
       </c>
       <c r="E23" s="3">
-        <v>5.5992802522620157E-2</v>
+        <v>4.8939566837508157E-2</v>
       </c>
       <c r="G23" s="12">
-        <f t="shared" si="10"/>
+        <f t="shared" si="5"/>
         <v>8.495760690496724E-9</v>
       </c>
       <c r="H23" s="12">
-        <f t="shared" si="11"/>
-        <v>7.8633069816233951E-10</v>
+        <f t="shared" si="5"/>
+        <v>7.0023727658747326E-9</v>
       </c>
       <c r="I23" s="12">
-        <f t="shared" si="12"/>
-        <v>1.0222749363738655E-9</v>
-      </c>
+        <f t="shared" si="5"/>
+        <v>8.6175681829971928E-9</v>
+      </c>
+      <c r="J23" s="3"/>
       <c r="K23" s="3">
-        <f t="shared" si="13"/>
-        <v>1.2218557880483052E-2</v>
+        <f t="shared" si="6"/>
+        <v>1.5344220925530401E-2</v>
       </c>
       <c r="L23" s="3">
-        <f t="shared" si="14"/>
-        <v>-1.5215953559437979E-2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+        <f t="shared" si="6"/>
+        <v>-1.1288380919373328E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" s="6" t="s">
         <v>43</v>
       </c>
@@ -15487,33 +15708,34 @@
         <v>5.299540684366523E-2</v>
       </c>
       <c r="D24" s="3">
-        <v>53146.211248178683</v>
+        <v>50850.386459921072</v>
       </c>
       <c r="E24" s="3">
-        <v>72977.814296823359</v>
+        <v>66096.082399088162</v>
       </c>
       <c r="G24" s="12">
-        <f t="shared" si="10"/>
+        <f t="shared" si="5"/>
         <v>8.495760690496724E-9</v>
       </c>
       <c r="H24" s="12">
-        <f t="shared" si="11"/>
-        <v>1.0248584296740678E-3</v>
+        <f t="shared" si="5"/>
+        <v>9.4571619086678636E-3</v>
       </c>
       <c r="I24" s="12">
-        <f t="shared" si="12"/>
-        <v>1.3323746464887225E-3</v>
-      </c>
+        <f t="shared" si="5"/>
+        <v>1.1638588845592334E-2</v>
+      </c>
+      <c r="J24" s="3"/>
       <c r="K24" s="3">
-        <f t="shared" si="13"/>
-        <v>-53146.158252771842</v>
+        <f t="shared" si="6"/>
+        <v>-50850.333464514231</v>
       </c>
       <c r="L24" s="3">
-        <f t="shared" si="14"/>
-        <v>-19831.603048644676</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+        <f t="shared" si="6"/>
+        <v>-15245.69593916709</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" s="6" t="s">
         <v>45</v>
       </c>
@@ -15524,33 +15746,34 @@
         <v>410905.13350763603</v>
       </c>
       <c r="D25" s="3">
-        <v>215410.71199267029</v>
+        <v>208522.9982026174</v>
       </c>
       <c r="E25" s="3">
-        <v>172466.39436131739</v>
+        <v>156202.99295912831</v>
       </c>
       <c r="G25" s="12">
-        <f t="shared" si="10"/>
+        <f t="shared" si="5"/>
         <v>6.5872721594074729E-2</v>
       </c>
       <c r="H25" s="12">
-        <f t="shared" si="11"/>
-        <v>4.1539270409486915E-3</v>
+        <f t="shared" si="5"/>
+        <v>3.8781136053652555E-2</v>
       </c>
       <c r="I25" s="12">
-        <f t="shared" si="12"/>
-        <v>3.1487631334602378E-3</v>
-      </c>
+        <f t="shared" si="5"/>
+        <v>2.7505146228263128E-2</v>
+      </c>
+      <c r="J25" s="3"/>
       <c r="K25" s="3">
-        <f t="shared" si="13"/>
-        <v>195494.42151496574</v>
+        <f t="shared" si="6"/>
+        <v>202382.13530501863</v>
       </c>
       <c r="L25" s="3">
-        <f t="shared" si="14"/>
-        <v>42944.317631352897</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+        <f t="shared" si="6"/>
+        <v>52320.005243489082</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26" s="6" t="s">
         <v>47</v>
       </c>
@@ -15561,33 +15784,34 @@
         <v>9.7158245880052951E-2</v>
       </c>
       <c r="D26" s="3">
-        <v>4.0776848963182177E-2</v>
+        <v>3.7651185918134829E-2</v>
       </c>
       <c r="E26" s="3">
-        <v>5.5992802522620157E-2</v>
+        <v>4.8939566837508157E-2</v>
       </c>
       <c r="G26" s="12">
-        <f t="shared" si="10"/>
+        <f t="shared" si="5"/>
         <v>1.5575561265910667E-8</v>
       </c>
       <c r="H26" s="12">
-        <f t="shared" si="11"/>
-        <v>7.8633069816233951E-10</v>
+        <f t="shared" si="5"/>
+        <v>7.0023727658747326E-9</v>
       </c>
       <c r="I26" s="12">
-        <f t="shared" si="12"/>
-        <v>1.0222749363738655E-9</v>
-      </c>
+        <f t="shared" si="5"/>
+        <v>8.6175681829971928E-9</v>
+      </c>
+      <c r="J26" s="3"/>
       <c r="K26" s="3">
-        <f t="shared" si="13"/>
-        <v>5.6381396916870774E-2</v>
+        <f t="shared" si="6"/>
+        <v>5.9507059961918123E-2</v>
       </c>
       <c r="L26" s="3">
-        <f t="shared" si="14"/>
-        <v>-1.5215953559437979E-2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+        <f t="shared" si="6"/>
+        <v>-1.1288380919373328E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" s="6" t="s">
         <v>49</v>
       </c>
@@ -15598,33 +15822,34 @@
         <v>-29268.92157136586</v>
       </c>
       <c r="D27" s="3">
-        <v>-6568.3034641824916</v>
+        <v>-11101.41451677614</v>
       </c>
       <c r="E27" s="3">
-        <v>-29559.797836237529</v>
+        <v>-27506.20621680946</v>
       </c>
       <c r="G27" s="12">
-        <f t="shared" si="10"/>
+        <f t="shared" si="5"/>
         <v>-4.6921378313555737E-3</v>
       </c>
       <c r="H27" s="12">
-        <f t="shared" si="11"/>
-        <v>-1.2666154399022185E-4</v>
+        <f t="shared" si="5"/>
+        <v>-2.0646426076453999E-3</v>
       </c>
       <c r="I27" s="12">
-        <f t="shared" si="12"/>
-        <v>-5.3968079986809706E-4</v>
-      </c>
+        <f t="shared" si="5"/>
+        <v>-4.8434553643672161E-3</v>
+      </c>
+      <c r="J27" s="3"/>
       <c r="K27" s="3">
-        <f t="shared" si="13"/>
-        <v>-22700.618107183367</v>
+        <f t="shared" si="6"/>
+        <v>-18167.507054589718</v>
       </c>
       <c r="L27" s="3">
-        <f t="shared" si="14"/>
-        <v>22991.494372055036</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.3">
+        <f t="shared" si="6"/>
+        <v>16404.791700033318</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
         <v>51</v>
       </c>
@@ -15635,37 +15860,44 @@
         <v>796661.85314938251</v>
       </c>
       <c r="D28" s="11">
-        <v>570160.71601398883</v>
+        <v>543131.55988495692</v>
       </c>
       <c r="E28" s="11">
-        <v>639051.47169947077</v>
+        <v>578055.71326794871</v>
       </c>
       <c r="G28" s="13">
-        <f t="shared" si="10"/>
+        <f t="shared" si="5"/>
         <v>0.12771386915796148</v>
       </c>
       <c r="H28" s="13">
-        <f t="shared" si="11"/>
-        <v>1.0994838622592571E-2</v>
+        <f t="shared" si="5"/>
+        <v>0.1010116826464596</v>
       </c>
       <c r="I28" s="13">
-        <f t="shared" si="12"/>
-        <v>1.1667326390874699E-2</v>
-      </c>
+        <f t="shared" si="5"/>
+        <v>0.10178746655435787</v>
+      </c>
+      <c r="J28" s="11"/>
       <c r="K28" s="11">
-        <f t="shared" si="13"/>
-        <v>226501.13713539368</v>
+        <f t="shared" si="6"/>
+        <v>253530.29326442559</v>
       </c>
       <c r="L28" s="11">
-        <f t="shared" si="14"/>
-        <v>-68890.755685481941</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+        <f t="shared" si="6"/>
+        <v>-34924.15338299179</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" s="4"/>
       <c r="B29" s="2"/>
-    </row>
-    <row r="30" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+      <c r="I29" s="3"/>
+      <c r="J29" s="3"/>
+      <c r="K29" s="3"/>
+      <c r="L29" s="3"/>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" s="6" t="s">
         <v>53</v>
       </c>
@@ -15676,33 +15908,34 @@
         <v>278338.39845116198</v>
       </c>
       <c r="D30" s="3">
-        <v>319711.06724665768</v>
+        <v>287205.4550950168</v>
       </c>
       <c r="E30" s="3">
-        <v>328010.04642499093</v>
+        <v>293802.11447809648</v>
       </c>
       <c r="G30" s="12">
-        <f t="shared" ref="G30:G34" si="15">C30/C$43</f>
+        <f t="shared" ref="G30:I34" si="7">C30/C$43</f>
         <v>4.4620780649783025E-2</v>
       </c>
       <c r="H30" s="12">
-        <f t="shared" ref="H30:H34" si="16">D30/D$43</f>
-        <v>6.1652293669204631E-3</v>
+        <f t="shared" si="7"/>
+        <v>5.3414510271755908E-2</v>
       </c>
       <c r="I30" s="12">
-        <f t="shared" ref="I30:I34" si="17">E30/E$43</f>
-        <v>5.9885634265874448E-3</v>
-      </c>
+        <f t="shared" si="7"/>
+        <v>5.1734412816324335E-2</v>
+      </c>
+      <c r="J30" s="3"/>
       <c r="K30" s="3">
-        <f t="shared" ref="K30:K34" si="18">C30-D30</f>
-        <v>-41372.668795495701</v>
+        <f t="shared" ref="K30:L34" si="8">C30-D30</f>
+        <v>-8867.0566438548267</v>
       </c>
       <c r="L30" s="3">
-        <f t="shared" ref="L30:L34" si="19">D30-E30</f>
-        <v>-8298.9791783332475</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+        <f t="shared" si="8"/>
+        <v>-6596.6593830796774</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31" s="6" t="s">
         <v>55</v>
       </c>
@@ -15713,33 +15946,34 @@
         <v>129319.67234919489</v>
       </c>
       <c r="D31" s="3">
-        <v>34685.711477594843</v>
+        <v>30847.55989102535</v>
       </c>
       <c r="E31" s="3">
-        <v>33040.406517582647</v>
+        <v>29251.519939833172</v>
       </c>
       <c r="G31" s="12">
-        <f t="shared" si="15"/>
+        <f t="shared" si="7"/>
         <v>2.073140021536668E-2</v>
       </c>
       <c r="H31" s="12">
-        <f t="shared" si="16"/>
-        <v>6.6887070521464244E-4</v>
+        <f t="shared" si="7"/>
+        <v>5.7370334561112867E-3</v>
       </c>
       <c r="I31" s="12">
-        <f t="shared" si="17"/>
-        <v>6.0322716400707682E-4</v>
-      </c>
+        <f t="shared" si="7"/>
+        <v>5.1507805202848263E-3</v>
+      </c>
+      <c r="J31" s="3"/>
       <c r="K31" s="3">
-        <f t="shared" si="18"/>
-        <v>94633.960871600051</v>
+        <f t="shared" si="8"/>
+        <v>98472.112458169548</v>
       </c>
       <c r="L31" s="3">
-        <f t="shared" si="19"/>
-        <v>1645.3049600121958</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+        <f t="shared" si="8"/>
+        <v>1596.0399511921787</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32" s="6" t="s">
         <v>57</v>
       </c>
@@ -15750,33 +15984,34 @@
         <v>5.5304050030874387E-2</v>
       </c>
       <c r="D32" s="3">
-        <v>7.5860086256153508E-2</v>
+        <v>6.4870941598969847E-2</v>
       </c>
       <c r="E32" s="3">
-        <v>7.181564591546423E-2</v>
+        <v>6.1357149498103267E-2</v>
       </c>
       <c r="G32" s="12">
-        <f t="shared" si="15"/>
+        <f t="shared" si="7"/>
         <v>8.8658621994092678E-9</v>
       </c>
       <c r="H32" s="12">
-        <f t="shared" si="16"/>
-        <v>1.4628671931545292E-9</v>
+        <f t="shared" si="7"/>
+        <v>1.2064706693089457E-8</v>
       </c>
       <c r="I32" s="12">
-        <f t="shared" si="17"/>
-        <v>1.3111566406989663E-9</v>
-      </c>
+        <f t="shared" si="7"/>
+        <v>1.0804129531220409E-8</v>
+      </c>
+      <c r="J32" s="3"/>
       <c r="K32" s="3">
-        <f t="shared" si="18"/>
-        <v>-2.0556036225279121E-2</v>
+        <f t="shared" si="8"/>
+        <v>-9.5668915680954605E-3</v>
       </c>
       <c r="L32" s="3">
-        <f t="shared" si="19"/>
-        <v>4.0444403406892787E-3</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+        <f t="shared" si="8"/>
+        <v>3.5137921008665807E-3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33" s="6" t="s">
         <v>59</v>
       </c>
@@ -15787,33 +16022,34 @@
         <v>433512.91697130748</v>
       </c>
       <c r="D33" s="3">
-        <v>17867.67623938687</v>
+        <v>15890.52637031726</v>
       </c>
       <c r="E33" s="3">
-        <v>43614.9731160511</v>
+        <v>38613.455167403263</v>
       </c>
       <c r="G33" s="12">
-        <f t="shared" si="15"/>
+        <f t="shared" si="7"/>
         <v>6.9497003951534936E-2</v>
       </c>
       <c r="H33" s="12">
-        <f t="shared" si="16"/>
-        <v>3.4455586169842401E-4</v>
+        <f t="shared" si="7"/>
+        <v>2.9553222927124214E-3</v>
       </c>
       <c r="I33" s="12">
-        <f t="shared" si="17"/>
-        <v>7.9628973472343698E-4</v>
-      </c>
+        <f t="shared" si="7"/>
+        <v>6.7992854082879672E-3</v>
+      </c>
+      <c r="J33" s="3"/>
       <c r="K33" s="3">
-        <f t="shared" si="18"/>
-        <v>415645.24073192058</v>
+        <f t="shared" si="8"/>
+        <v>417622.39060099021</v>
       </c>
       <c r="L33" s="3">
-        <f t="shared" si="19"/>
-        <v>-25747.29687666423</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.3">
+        <f t="shared" si="8"/>
+        <v>-22722.928797086002</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="4" t="s">
         <v>61</v>
       </c>
@@ -15824,37 +16060,44 @@
         <v>841171.04307571449</v>
       </c>
       <c r="D34" s="11">
-        <v>372264.53082372562</v>
+        <v>333943.606227301</v>
       </c>
       <c r="E34" s="11">
-        <v>404665.49787427048</v>
+        <v>361667.1509424824</v>
       </c>
       <c r="G34" s="13">
-        <f t="shared" si="15"/>
+        <f t="shared" si="7"/>
         <v>0.13484919368254686</v>
       </c>
       <c r="H34" s="13">
-        <f t="shared" si="16"/>
-        <v>7.1786573967007224E-3</v>
+        <f t="shared" si="7"/>
+        <v>6.210687808528631E-2</v>
       </c>
       <c r="I34" s="13">
-        <f t="shared" si="17"/>
-        <v>7.3880816364745973E-3</v>
-      </c>
+        <f t="shared" si="7"/>
+        <v>6.3684489549026654E-2</v>
+      </c>
+      <c r="J34" s="11"/>
       <c r="K34" s="11">
-        <f t="shared" si="18"/>
-        <v>468906.51225198887</v>
+        <f t="shared" si="8"/>
+        <v>507227.43684841349</v>
       </c>
       <c r="L34" s="11">
-        <f t="shared" si="19"/>
-        <v>-32400.967050544859</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+        <f t="shared" si="8"/>
+        <v>-27723.544715181401</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A35" s="4"/>
       <c r="B35" s="2"/>
-    </row>
-    <row r="36" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G35" s="3"/>
+      <c r="H35" s="3"/>
+      <c r="I35" s="3"/>
+      <c r="J35" s="3"/>
+      <c r="K35" s="3"/>
+      <c r="L35" s="3"/>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A36" s="6" t="s">
         <v>53</v>
       </c>
@@ -15865,33 +16108,34 @@
         <v>28013.675515786948</v>
       </c>
       <c r="D36" s="3">
-        <v>36157.500071022012</v>
+        <v>31929.81009177423</v>
       </c>
       <c r="E36" s="3">
-        <v>28294.164336895479</v>
+        <v>24844.53207040147</v>
       </c>
       <c r="G36" s="12">
-        <f t="shared" ref="G36:G41" si="20">C36/C$43</f>
+        <f t="shared" ref="G36:I41" si="9">C36/C$43</f>
         <v>4.490907748768461E-3</v>
       </c>
       <c r="H36" s="12">
-        <f t="shared" ref="H36:H41" si="21">D36/D$43</f>
-        <v>6.9725231344685049E-4</v>
+        <f t="shared" si="9"/>
+        <v>5.9383104981695104E-3</v>
       </c>
       <c r="I36" s="12">
-        <f t="shared" ref="I36:I41" si="22">E36/E$43</f>
-        <v>5.1657380492013314E-4</v>
-      </c>
+        <f t="shared" si="9"/>
+        <v>4.3747720490091352E-3</v>
+      </c>
+      <c r="J36" s="3"/>
       <c r="K36" s="3">
-        <f t="shared" ref="K36:K41" si="23">C36-D36</f>
-        <v>-8143.8245552350636</v>
+        <f t="shared" ref="K36:L41" si="10">C36-D36</f>
+        <v>-3916.134575987282</v>
       </c>
       <c r="L36" s="3">
-        <f t="shared" ref="L36:L41" si="24">D36-E36</f>
-        <v>7863.3357341265328</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+        <f t="shared" si="10"/>
+        <v>7085.2780213727601</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37" s="6" t="s">
         <v>64</v>
       </c>
@@ -15902,33 +16146,34 @@
         <v>4546699.7209444745</v>
       </c>
       <c r="D37" s="3">
-        <v>50852555.932043023</v>
+        <v>4444977.9171573538</v>
       </c>
       <c r="E37" s="3">
-        <v>53675441.835535713</v>
+        <v>4692208.1520119831</v>
       </c>
       <c r="G37" s="12">
-        <f t="shared" si="20"/>
+        <f t="shared" si="9"/>
         <v>0.72888718214095238</v>
       </c>
       <c r="H37" s="12">
-        <f t="shared" si="21"/>
-        <v>0.98062814626719697</v>
+        <f t="shared" si="9"/>
+        <v>0.82667760796946355</v>
       </c>
       <c r="I37" s="12">
-        <f t="shared" si="22"/>
-        <v>0.9799662887938928</v>
-      </c>
+        <f t="shared" si="9"/>
+        <v>0.82623174440906766</v>
+      </c>
+      <c r="J37" s="3"/>
       <c r="K37" s="3">
-        <f t="shared" si="23"/>
-        <v>-46305856.211098552</v>
+        <f t="shared" si="10"/>
+        <v>101721.80378712062</v>
       </c>
       <c r="L37" s="3">
-        <f t="shared" si="24"/>
-        <v>-2822885.9034926891</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+        <f t="shared" si="10"/>
+        <v>-247230.23485462926</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A38" s="6" t="s">
         <v>66</v>
       </c>
@@ -15939,33 +16184,34 @@
         <v>7869.2833005095372</v>
       </c>
       <c r="D38" s="3">
-        <v>9251.8577164824183</v>
+        <v>8093.9719745525617</v>
       </c>
       <c r="E38" s="3">
-        <v>9245.5644064244752</v>
+        <v>8088.9283763771145</v>
       </c>
       <c r="G38" s="12">
-        <f t="shared" si="20"/>
+        <f t="shared" si="9"/>
         <v>1.2615347576078243E-3</v>
       </c>
       <c r="H38" s="12">
-        <f t="shared" si="21"/>
-        <v>1.7841054231701266E-4</v>
+        <f t="shared" si="9"/>
+        <v>1.50531802758068E-3</v>
       </c>
       <c r="I38" s="12">
-        <f t="shared" si="22"/>
-        <v>1.6879863731592655E-4</v>
-      </c>
+        <f t="shared" si="9"/>
+        <v>1.4243463176177105E-3</v>
+      </c>
+      <c r="J38" s="3"/>
       <c r="K38" s="3">
-        <f t="shared" si="23"/>
-        <v>-1382.5744159728811</v>
+        <f t="shared" si="10"/>
+        <v>-224.68867404302455</v>
       </c>
       <c r="L38" s="3">
-        <f t="shared" si="24"/>
-        <v>6.2933100579430175</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+        <f t="shared" si="10"/>
+        <v>5.0435981754471868</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A39" s="6" t="s">
         <v>57</v>
       </c>
@@ -15976,33 +16222,34 @@
         <v>6127.3618318472836</v>
       </c>
       <c r="D39" s="3">
-        <v>6224.4582277989939</v>
+        <v>5520.4629756121931</v>
       </c>
       <c r="E39" s="3">
-        <v>5542.1996189579158</v>
+        <v>4866.4931232556364</v>
       </c>
       <c r="G39" s="12">
-        <f t="shared" si="20"/>
+        <f t="shared" si="9"/>
         <v>9.8228512408676219E-4</v>
       </c>
       <c r="H39" s="12">
-        <f t="shared" si="21"/>
-        <v>1.2003091725814269E-4</v>
+        <f t="shared" si="9"/>
+        <v>1.0266964679279237E-3</v>
       </c>
       <c r="I39" s="12">
-        <f t="shared" si="22"/>
-        <v>1.0118535789582307E-4</v>
-      </c>
+        <f t="shared" si="9"/>
+        <v>8.5692087224607165E-4</v>
+      </c>
+      <c r="J39" s="3"/>
       <c r="K39" s="3">
-        <f t="shared" si="23"/>
-        <v>-97.096395951710292</v>
+        <f t="shared" si="10"/>
+        <v>606.89885623509053</v>
       </c>
       <c r="L39" s="3">
-        <f t="shared" si="24"/>
-        <v>682.25860884107806</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+        <f t="shared" si="10"/>
+        <v>653.96985235655666</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A40" s="6" t="s">
         <v>59</v>
       </c>
@@ -16013,33 +16260,34 @@
         <v>11321.895515618429</v>
       </c>
       <c r="D40" s="3">
-        <v>10509.56920654072</v>
+        <v>9320.9216884499019</v>
       </c>
       <c r="E40" s="3">
-        <v>10502.420374423</v>
+        <v>9315.1135408841401</v>
       </c>
       <c r="G40" s="12">
-        <f t="shared" si="20"/>
+        <f t="shared" si="9"/>
         <v>1.8150273880763682E-3</v>
       </c>
       <c r="H40" s="12">
-        <f t="shared" si="21"/>
-        <v>2.0266394048805081E-4</v>
+        <f t="shared" si="9"/>
+        <v>1.7335063051125805E-3</v>
       </c>
       <c r="I40" s="12">
-        <f t="shared" si="22"/>
-        <v>1.9174537862607521E-4</v>
-      </c>
+        <f t="shared" si="9"/>
+        <v>1.6402602486748278E-3</v>
+      </c>
+      <c r="J40" s="3"/>
       <c r="K40" s="3">
-        <f t="shared" si="23"/>
-        <v>812.32630907770908</v>
+        <f t="shared" si="10"/>
+        <v>2000.9738271685274</v>
       </c>
       <c r="L40" s="3">
-        <f t="shared" si="24"/>
-        <v>7.1488321177203034</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.3">
+        <f t="shared" si="10"/>
+        <v>5.8081475657618284</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A41" s="4" t="s">
         <v>70</v>
       </c>
@@ -16050,37 +16298,44 @@
         <v>4600031.9371082364</v>
       </c>
       <c r="D41" s="11">
-        <v>50914699.317264847</v>
+        <v>4499843.0838877419</v>
       </c>
       <c r="E41" s="11">
-        <v>53729026.184272408</v>
+        <v>4739323.2191229016</v>
       </c>
       <c r="G41" s="13">
-        <f t="shared" si="20"/>
+        <f t="shared" si="9"/>
         <v>0.73743693715949177</v>
       </c>
       <c r="H41" s="13">
-        <f t="shared" si="21"/>
-        <v>0.98182650398070659</v>
+        <f t="shared" si="9"/>
+        <v>0.83688143926825409</v>
       </c>
       <c r="I41" s="13">
-        <f t="shared" si="22"/>
-        <v>0.9809445919726506</v>
-      </c>
+        <f t="shared" si="9"/>
+        <v>0.83452804389661539</v>
+      </c>
+      <c r="J41" s="11"/>
       <c r="K41" s="11">
-        <f t="shared" si="23"/>
-        <v>-46314667.380156614</v>
+        <f t="shared" si="10"/>
+        <v>100188.85322049446</v>
       </c>
       <c r="L41" s="11">
-        <f t="shared" si="24"/>
-        <v>-2814326.867007561</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+        <f t="shared" si="10"/>
+        <v>-239480.13523515966</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A42" s="4"/>
       <c r="B42" s="2"/>
-    </row>
-    <row r="43" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G42" s="3"/>
+      <c r="H42" s="3"/>
+      <c r="I42" s="3"/>
+      <c r="J42" s="3"/>
+      <c r="K42" s="3"/>
+      <c r="L42" s="3"/>
+    </row>
+    <row r="43" spans="1:12" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A43" s="4" t="s">
         <v>72</v>
       </c>
@@ -16091,21 +16346,25 @@
         <v>6237864.833333333</v>
       </c>
       <c r="D43" s="11">
-        <v>51857124.564102568</v>
+        <v>5376918.25</v>
       </c>
       <c r="E43" s="11">
-        <v>54772743.153846152</v>
-      </c>
+        <v>5679046.083333333</v>
+      </c>
+      <c r="G43" s="11"/>
+      <c r="H43" s="11"/>
+      <c r="I43" s="11"/>
+      <c r="J43" s="11"/>
       <c r="K43" s="11">
-        <f t="shared" ref="K43:K63" si="25">C43-D43</f>
-        <v>-45619259.730769232</v>
+        <f t="shared" ref="K43:L63" si="11">C43-D43</f>
+        <v>860946.58333333302</v>
       </c>
       <c r="L43" s="11">
-        <f t="shared" ref="L43:L44" si="26">D43-E43</f>
-        <v>-2915618.5897435844</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.3">
+        <f t="shared" si="11"/>
+        <v>-302127.83333333302</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A44" s="4" t="s">
         <v>74</v>
       </c>
@@ -16116,25 +16375,35 @@
         <v>6237864.833333333</v>
       </c>
       <c r="D44" s="11">
-        <v>51857124.564102568</v>
+        <v>5376918.25</v>
       </c>
       <c r="E44" s="11">
-        <v>54772743.153846152</v>
-      </c>
+        <v>5679046.083333333</v>
+      </c>
+      <c r="G44" s="11"/>
+      <c r="H44" s="11"/>
+      <c r="I44" s="11"/>
+      <c r="J44" s="11"/>
       <c r="K44" s="11">
-        <f t="shared" si="25"/>
-        <v>-45619259.730769232</v>
+        <f t="shared" si="11"/>
+        <v>860946.58333333302</v>
       </c>
       <c r="L44" s="11">
-        <f t="shared" si="26"/>
-        <v>-2915618.5897435844</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+        <f t="shared" si="11"/>
+        <v>-302127.83333333302</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A45" s="4"/>
       <c r="B45" s="2"/>
-    </row>
-    <row r="46" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G45" s="3"/>
+      <c r="H45" s="3"/>
+      <c r="I45" s="3"/>
+      <c r="J45" s="3"/>
+      <c r="K45" s="3"/>
+      <c r="L45" s="3"/>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A46" s="6" t="s">
         <v>76</v>
       </c>
@@ -16145,22 +16414,28 @@
         <v>232572.25000000029</v>
       </c>
       <c r="D46" s="3">
-        <v>148943.15384615649</v>
+        <v>161355.08333333331</v>
+      </c>
+      <c r="E46" s="3">
+        <v>0</v>
       </c>
       <c r="G46" s="12">
         <f>C$63/C46</f>
         <v>6.1334703516864035E-2</v>
       </c>
       <c r="H46" s="12">
-        <f t="shared" ref="H46:H48" si="27">D$63/D46</f>
-        <v>-2.9877686944063311E-2</v>
-      </c>
+        <f t="shared" ref="H46:H48" si="12">D$63/D46</f>
+        <v>-2.9849798141882739E-2</v>
+      </c>
+      <c r="I46" s="3"/>
+      <c r="J46" s="3"/>
       <c r="K46" s="3">
-        <f t="shared" si="25"/>
-        <v>83629.096153843799</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+        <f t="shared" si="11"/>
+        <v>71217.166666666977</v>
+      </c>
+      <c r="L46" s="3"/>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A47" s="6" t="s">
         <v>78</v>
       </c>
@@ -16171,22 +16446,28 @@
         <v>293072.00000000029</v>
       </c>
       <c r="D47" s="3">
-        <v>138707.8461538486</v>
+        <v>150266.83333333331</v>
+      </c>
+      <c r="E47" s="3">
+        <v>0</v>
       </c>
       <c r="G47" s="12">
-        <f t="shared" ref="G47:G48" si="28">C$63/C47</f>
+        <f t="shared" ref="G47:G48" si="13">C$63/C47</f>
         <v>4.8673192935524329E-2</v>
       </c>
       <c r="H47" s="12">
-        <f t="shared" si="27"/>
-        <v>-3.2082373466754681E-2</v>
-      </c>
+        <f t="shared" si="12"/>
+        <v>-3.205242673865713E-2</v>
+      </c>
+      <c r="I47" s="3"/>
+      <c r="J47" s="3"/>
       <c r="K47" s="3">
-        <f t="shared" si="25"/>
-        <v>154364.15384615169</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.3">
+        <f t="shared" si="11"/>
+        <v>142805.16666666698</v>
+      </c>
+      <c r="L47" s="3"/>
+    </row>
+    <row r="48" spans="1:12" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A48" s="4" t="s">
         <v>80</v>
       </c>
@@ -16197,26 +16478,38 @@
         <v>-60499.750000000073</v>
       </c>
       <c r="D48" s="11">
-        <v>10235.307692307861</v>
+        <v>11088.25</v>
+      </c>
+      <c r="E48" s="11">
+        <v>0</v>
       </c>
       <c r="G48" s="14">
-        <f t="shared" si="28"/>
+        <f t="shared" si="13"/>
         <v>-0.23578196604118171</v>
       </c>
       <c r="H48" s="14">
-        <f t="shared" si="27"/>
-        <v>-0.434777053788162</v>
-      </c>
+        <f t="shared" si="12"/>
+        <v>-0.43437121878264534</v>
+      </c>
+      <c r="I48" s="11"/>
+      <c r="J48" s="11"/>
       <c r="K48" s="11">
-        <f t="shared" si="25"/>
-        <v>-70735.057692307935</v>
-      </c>
-    </row>
-    <row r="49" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
+        <f t="shared" si="11"/>
+        <v>-71588.000000000073</v>
+      </c>
+      <c r="L48" s="11"/>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A49" s="4"/>
       <c r="B49" s="2"/>
-    </row>
-    <row r="50" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G49" s="3"/>
+      <c r="H49" s="3"/>
+      <c r="I49" s="3"/>
+      <c r="J49" s="3"/>
+      <c r="K49" s="3"/>
+      <c r="L49" s="3"/>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A50" s="6" t="s">
         <v>82</v>
       </c>
@@ -16227,22 +16520,28 @@
         <v>1000.3333333333341</v>
       </c>
       <c r="D50" s="3">
-        <v>857.00000000001467</v>
+        <v>928.41666666666663</v>
+      </c>
+      <c r="E50" s="3">
+        <v>0</v>
       </c>
       <c r="G50" s="12">
-        <f t="shared" ref="G50:G52" si="29">C$63/C50</f>
+        <f t="shared" ref="G50:H52" si="14">C$63/C50</f>
         <v>14.259996667777397</v>
       </c>
       <c r="H50" s="12">
-        <f t="shared" ref="H50:H52" si="30">D$63/D50</f>
-        <v>-5.1926218472308596</v>
-      </c>
+        <f t="shared" si="14"/>
+        <v>-5.1877748855578503</v>
+      </c>
+      <c r="I50" s="3"/>
+      <c r="J50" s="3"/>
       <c r="K50" s="3">
-        <f t="shared" si="25"/>
-        <v>143.33333333331939</v>
-      </c>
-    </row>
-    <row r="51" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
+        <f t="shared" si="11"/>
+        <v>71.916666666667425</v>
+      </c>
+      <c r="L50" s="3"/>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A51" s="10" t="s">
         <v>84</v>
       </c>
@@ -16253,22 +16552,28 @@
         <v>26254.083333333361</v>
       </c>
       <c r="D51" s="3">
-        <v>72639.307692308925</v>
+        <v>78689.083333333328</v>
+      </c>
+      <c r="E51" s="3">
+        <v>0</v>
       </c>
       <c r="G51" s="12">
-        <f t="shared" si="29"/>
+        <f t="shared" si="14"/>
         <v>0.54333452891454925</v>
       </c>
       <c r="H51" s="12">
-        <f t="shared" si="30"/>
-        <v>-6.1262656052930672E-2</v>
-      </c>
+        <f t="shared" si="14"/>
+        <v>-6.1208193851540194E-2</v>
+      </c>
+      <c r="I51" s="3"/>
+      <c r="J51" s="3"/>
       <c r="K51" s="3">
-        <f t="shared" si="25"/>
-        <v>-46385.224358975567</v>
-      </c>
-    </row>
-    <row r="52" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.3">
+        <f t="shared" si="11"/>
+        <v>-52434.999999999971</v>
+      </c>
+      <c r="L51" s="3"/>
+    </row>
+    <row r="52" spans="1:12" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A52" s="9" t="s">
         <v>105</v>
       </c>
@@ -16279,26 +16584,38 @@
         <v>-87754.166666666759</v>
       </c>
       <c r="D52" s="11">
-        <v>-63261.000000001077</v>
+        <v>-68529.25</v>
+      </c>
+      <c r="E52" s="11">
+        <v>0</v>
       </c>
       <c r="G52" s="14">
-        <f t="shared" si="29"/>
+        <f t="shared" si="14"/>
         <v>-0.16255353496984931</v>
       </c>
       <c r="H52" s="14">
-        <f t="shared" si="30"/>
-        <v>7.0344713537200593E-2</v>
-      </c>
+        <f t="shared" si="14"/>
+        <v>7.0282640867464136E-2</v>
+      </c>
+      <c r="I52" s="11"/>
+      <c r="J52" s="11"/>
       <c r="K52" s="11">
-        <f t="shared" si="25"/>
-        <v>-24493.166666665682</v>
-      </c>
-    </row>
-    <row r="53" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
+        <f t="shared" si="11"/>
+        <v>-19224.916666666759</v>
+      </c>
+      <c r="L52" s="11"/>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A53" s="5"/>
       <c r="B53" s="2"/>
-    </row>
-    <row r="54" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G53" s="3"/>
+      <c r="H53" s="3"/>
+      <c r="I53" s="3"/>
+      <c r="J53" s="3"/>
+      <c r="K53" s="3"/>
+      <c r="L53" s="3"/>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A54" s="6" t="s">
         <v>87</v>
       </c>
@@ -16311,20 +16628,26 @@
       <c r="D54" s="3">
         <v>0</v>
       </c>
+      <c r="E54" s="3">
+        <v>0</v>
+      </c>
       <c r="G54" s="12" t="e">
-        <f t="shared" ref="G54:G59" si="31">C$63/C54</f>
+        <f t="shared" ref="G54:H59" si="15">C$63/C54</f>
         <v>#DIV/0!</v>
       </c>
       <c r="H54" s="12" t="e">
-        <f t="shared" ref="H54:H59" si="32">D$63/D54</f>
+        <f t="shared" si="15"/>
         <v>#DIV/0!</v>
       </c>
+      <c r="I54" s="3"/>
+      <c r="J54" s="3"/>
       <c r="K54" s="3">
-        <f t="shared" si="25"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="L54" s="3"/>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A55" s="6" t="s">
         <v>89</v>
       </c>
@@ -16335,22 +16658,28 @@
         <v>2448.7500000000032</v>
       </c>
       <c r="D55" s="3">
-        <v>7437.0000000001264</v>
+        <v>8056.75</v>
+      </c>
+      <c r="E55" s="3">
+        <v>0</v>
       </c>
       <c r="G55" s="12">
-        <f t="shared" si="31"/>
+        <f t="shared" si="15"/>
         <v>5.8253190403266899</v>
       </c>
       <c r="H55" s="12">
-        <f t="shared" si="32"/>
-        <v>-0.59836989687734932</v>
-      </c>
+        <f t="shared" si="15"/>
+        <v>-0.59781135900538884</v>
+      </c>
+      <c r="I55" s="3"/>
+      <c r="J55" s="3"/>
       <c r="K55" s="3">
-        <f t="shared" si="25"/>
-        <v>-4988.2500000001237</v>
-      </c>
-    </row>
-    <row r="56" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
+        <f t="shared" si="11"/>
+        <v>-5607.9999999999964</v>
+      </c>
+      <c r="L55" s="3"/>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A56" s="6" t="s">
         <v>91</v>
       </c>
@@ -16361,22 +16690,28 @@
         <v>24435.08333333335</v>
       </c>
       <c r="D56" s="3">
-        <v>8570.0000000001455</v>
+        <v>9284.1666666666661</v>
+      </c>
+      <c r="E56" s="3">
+        <v>0</v>
       </c>
       <c r="G56" s="12">
-        <f t="shared" si="31"/>
+        <f t="shared" si="15"/>
         <v>0.58378151633068531</v>
       </c>
       <c r="H56" s="12">
-        <f t="shared" si="32"/>
-        <v>-0.51926218472308605</v>
-      </c>
+        <f t="shared" si="15"/>
+        <v>-0.51877748855578498</v>
+      </c>
+      <c r="I56" s="3"/>
+      <c r="J56" s="3"/>
       <c r="K56" s="3">
-        <f t="shared" si="25"/>
-        <v>15865.083333333205</v>
-      </c>
-    </row>
-    <row r="57" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
+        <f t="shared" si="11"/>
+        <v>15150.916666666684</v>
+      </c>
+      <c r="L56" s="3"/>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A57" s="6" t="s">
         <v>93</v>
       </c>
@@ -16387,22 +16722,28 @@
         <v>220273.58333333349</v>
       </c>
       <c r="D57" s="3">
-        <v>257887.84615385061</v>
+        <v>279378.5</v>
+      </c>
+      <c r="E57" s="3">
+        <v>0</v>
       </c>
       <c r="G57" s="12">
-        <f t="shared" si="31"/>
+        <f t="shared" si="15"/>
         <v>6.4759240686676336E-2</v>
       </c>
       <c r="H57" s="12">
-        <f t="shared" si="32"/>
-        <v>-1.7255861373250209E-2</v>
-      </c>
+        <f t="shared" si="15"/>
+        <v>-1.7239754192490356E-2</v>
+      </c>
+      <c r="I57" s="3"/>
+      <c r="J57" s="3"/>
       <c r="K57" s="3">
-        <f t="shared" si="25"/>
-        <v>-37614.26282051712</v>
-      </c>
-    </row>
-    <row r="58" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
+        <f t="shared" si="11"/>
+        <v>-59104.916666666511</v>
+      </c>
+      <c r="L57" s="3"/>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A58" s="6" t="s">
         <v>95</v>
       </c>
@@ -16413,22 +16754,28 @@
         <v>90002.500000000087</v>
       </c>
       <c r="D58" s="3">
-        <v>199108.46153846491</v>
+        <v>215699.83333333331</v>
+      </c>
+      <c r="E58" s="3">
+        <v>0</v>
       </c>
       <c r="G58" s="12">
-        <f t="shared" si="31"/>
+        <f t="shared" si="15"/>
         <v>0.15849281964389864</v>
       </c>
       <c r="H58" s="12">
-        <f t="shared" si="32"/>
-        <v>-2.2350014101320509E-2</v>
-      </c>
+        <f t="shared" si="15"/>
+        <v>-2.2329255392717816E-2</v>
+      </c>
+      <c r="I58" s="3"/>
+      <c r="J58" s="3"/>
       <c r="K58" s="3">
-        <f t="shared" si="25"/>
-        <v>-109105.96153846482</v>
-      </c>
-    </row>
-    <row r="59" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.3">
+        <f t="shared" si="11"/>
+        <v>-125697.33333333323</v>
+      </c>
+      <c r="L58" s="3"/>
+    </row>
+    <row r="59" spans="1:12" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A59" s="4" t="s">
         <v>97</v>
       </c>
@@ -16439,26 +16786,38 @@
         <v>20530.583333333339</v>
       </c>
       <c r="D59" s="11">
-        <v>-5614.6153846153838</v>
+        <v>-6078</v>
+      </c>
+      <c r="E59" s="11">
+        <v>0</v>
       </c>
       <c r="G59" s="14">
-        <f t="shared" si="31"/>
+        <f t="shared" si="15"/>
         <v>0.69480490487768232</v>
       </c>
       <c r="H59" s="14">
-        <f t="shared" si="32"/>
-        <v>0.79258802575695309</v>
-      </c>
+        <f t="shared" si="15"/>
+        <v>0.79243446309092913</v>
+      </c>
+      <c r="I59" s="11"/>
+      <c r="J59" s="11"/>
       <c r="K59" s="11">
-        <f t="shared" si="25"/>
-        <v>26145.198717948722</v>
-      </c>
-    </row>
-    <row r="60" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
+        <f t="shared" si="11"/>
+        <v>26608.583333333339</v>
+      </c>
+      <c r="L59" s="11"/>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A60" s="4"/>
       <c r="B60" s="2"/>
-    </row>
-    <row r="61" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G60" s="3"/>
+      <c r="H60" s="3"/>
+      <c r="I60" s="3"/>
+      <c r="J60" s="3"/>
+      <c r="K60" s="3"/>
+      <c r="L60" s="3"/>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A61" s="6" t="s">
         <v>99</v>
       </c>
@@ -16469,22 +16828,28 @@
         <v>-6265.8333333333348</v>
       </c>
       <c r="D61" s="3">
-        <v>1164.538461538461</v>
+        <v>1261.583333333333</v>
+      </c>
+      <c r="E61" s="3">
+        <v>0</v>
       </c>
       <c r="G61" s="12">
-        <f t="shared" ref="G61:G63" si="33">C$63/C61</f>
+        <f t="shared" ref="G61:H63" si="16">C$63/C61</f>
         <v>-2.2765926319989354</v>
       </c>
       <c r="H61" s="12">
-        <f t="shared" ref="H61:H63" si="34">D$63/D61</f>
-        <v>-3.821322412312572</v>
-      </c>
+        <f t="shared" si="16"/>
+        <v>-3.8177554660149293</v>
+      </c>
+      <c r="I61" s="3"/>
+      <c r="J61" s="3"/>
       <c r="K61" s="3">
-        <f t="shared" si="25"/>
-        <v>-7430.3717948717958</v>
-      </c>
-    </row>
-    <row r="62" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
+        <f t="shared" si="11"/>
+        <v>-7527.4166666666679</v>
+      </c>
+      <c r="L61" s="3"/>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A62" s="6" t="s">
         <v>101</v>
       </c>
@@ -16497,20 +16862,26 @@
       <c r="D62" s="3">
         <v>0</v>
       </c>
+      <c r="E62" s="3">
+        <v>0</v>
+      </c>
       <c r="G62" s="12" t="e">
-        <f t="shared" si="33"/>
+        <f t="shared" si="16"/>
         <v>#DIV/0!</v>
       </c>
       <c r="H62" s="12" t="e">
-        <f t="shared" si="34"/>
+        <f t="shared" si="16"/>
         <v>#DIV/0!</v>
       </c>
+      <c r="I62" s="3"/>
+      <c r="J62" s="3"/>
       <c r="K62" s="3">
-        <f t="shared" si="25"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.3">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="L62" s="3"/>
+    </row>
+    <row r="63" spans="1:12" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A63" s="4" t="s">
         <v>103</v>
       </c>
@@ -16521,174 +16892,26 @@
         <v>14264.75</v>
       </c>
       <c r="D63" s="11">
-        <v>-4450.0769230769229</v>
+        <v>-4816.416666666667</v>
+      </c>
+      <c r="E63" s="11">
+        <v>0</v>
       </c>
       <c r="G63" s="14">
-        <f t="shared" si="33"/>
+        <f t="shared" si="16"/>
         <v>1</v>
       </c>
       <c r="H63" s="14">
-        <f t="shared" si="34"/>
+        <f t="shared" si="16"/>
         <v>1</v>
       </c>
+      <c r="I63" s="11"/>
+      <c r="J63" s="11"/>
       <c r="K63" s="11">
-        <f t="shared" si="25"/>
-        <v>18714.826923076922</v>
-      </c>
-    </row>
-    <row r="66" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C66" s="15">
-        <f>SUM(C3:C11)-C12</f>
-        <v>0</v>
-      </c>
-      <c r="D66" s="15">
-        <f t="shared" ref="D66:E66" si="35">SUM(D3:D11)-D12</f>
-        <v>0</v>
-      </c>
-      <c r="E66" s="15">
-        <f t="shared" si="35"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C67" s="15">
-        <f>SUM(C14:C19)-C20</f>
-        <v>0</v>
-      </c>
-      <c r="D67" s="15">
-        <f t="shared" ref="D67:E67" si="36">SUM(D14:D19)-D20</f>
-        <v>0</v>
-      </c>
-      <c r="E67" s="15">
-        <f t="shared" si="36"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C68" s="15">
-        <f>SUM(C22:C27)-C28</f>
-        <v>0</v>
-      </c>
-      <c r="D68" s="15">
-        <f t="shared" ref="D68:E68" si="37">SUM(D22:D27)-D28</f>
-        <v>0</v>
-      </c>
-      <c r="E68" s="15">
-        <f t="shared" si="37"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C69" s="15">
-        <f>SUM(C30:C33)-C34</f>
-        <v>0</v>
-      </c>
-      <c r="D69" s="15">
-        <f t="shared" ref="D69:E69" si="38">SUM(D30:D33)-D34</f>
-        <v>0</v>
-      </c>
-      <c r="E69" s="15">
-        <f t="shared" si="38"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="70" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C70" s="15">
-        <f>SUM(C36:C40)-C41</f>
-        <v>0</v>
-      </c>
-      <c r="D70" s="15">
-        <f t="shared" ref="D70:E70" si="39">SUM(D36:D40)-D41</f>
-        <v>0</v>
-      </c>
-      <c r="E70" s="15">
-        <f t="shared" si="39"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="71" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C71" s="15">
-        <f>SUM(C12,C20)-C43</f>
-        <v>0</v>
-      </c>
-      <c r="D71" s="15">
-        <f t="shared" ref="D71:E71" si="40">SUM(D12,D20)-D43</f>
-        <v>0</v>
-      </c>
-      <c r="E71" s="15">
-        <f t="shared" si="40"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="72" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C72" s="15">
-        <f>SUM(C28,C34,C41)-C44</f>
-        <v>0</v>
-      </c>
-      <c r="D72" s="15">
-        <f t="shared" ref="D72:E72" si="41">SUM(D28,D34,D41)-D44</f>
-        <v>0</v>
-      </c>
-      <c r="E72" s="15">
-        <f t="shared" si="41"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="73" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C73" s="15">
-        <f>C46-C47-C48</f>
-        <v>7.2759576141834259E-11</v>
-      </c>
-      <c r="D73" s="15">
-        <f t="shared" ref="D73:E73" si="42">D46-D47-D48</f>
-        <v>3.092281986027956E-11</v>
-      </c>
-      <c r="E73" s="15">
-        <f t="shared" si="42"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="74" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C74" s="15">
-        <f>C48-C50-C51-C52</f>
-        <v>0</v>
-      </c>
-      <c r="D74" s="15">
-        <f t="shared" ref="D74:E74" si="43">D48-D50-D51-D52</f>
-        <v>0</v>
-      </c>
-      <c r="E74" s="15">
-        <f t="shared" si="43"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="75" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C75" s="15">
-        <f>C52+C54+C55-C56+C57-C58-C59</f>
-        <v>-5.4569682106375694E-11</v>
-      </c>
-      <c r="D75" s="15">
-        <f t="shared" ref="D75:E75" si="44">D52+D54+D55-D56+D57-D58-D59</f>
-        <v>-2.0918378140777349E-11</v>
-      </c>
-      <c r="E75" s="15">
-        <f t="shared" si="44"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="76" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C76" s="15">
-        <f>C59+C61+C62-C63</f>
-        <v>0</v>
-      </c>
-      <c r="D76" s="15">
-        <f t="shared" ref="D76:E76" si="45">D59+D61+D62-D63</f>
-        <v>0</v>
-      </c>
-      <c r="E76" s="15">
-        <f t="shared" si="45"/>
-        <v>0</v>
-      </c>
+        <f t="shared" si="11"/>
+        <v>19081.166666666668</v>
+      </c>
+      <c r="L63" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>